<commit_message>
update the excel file with the results now all combinations have at least 50,100,150 and 250MHz tests
</commit_message>
<xml_diff>
--- a/results/Zynq7000_HPS-FPGA.xlsx
+++ b/results/Zynq7000_HPS-FPGA.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="45" yWindow="90" windowWidth="18915" windowHeight="7680"/>
+    <workbookView xWindow="45" yWindow="150" windowWidth="18915" windowHeight="7620"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -678,8 +678,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BO54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="BF40" sqref="BF40"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="BF52" sqref="BF52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1149,7 +1149,9 @@
       <c r="C9" s="2">
         <v>2</v>
       </c>
-      <c r="D9" s="4"/>
+      <c r="D9" s="4">
+        <v>0.98724049317417195</v>
+      </c>
       <c r="E9" s="5"/>
       <c r="F9" s="5">
         <v>1.0249052298831274</v>
@@ -1166,7 +1168,9 @@
       <c r="L9" s="6">
         <v>1.0360394529128192</v>
       </c>
-      <c r="M9" s="4"/>
+      <c r="M9" s="4">
+        <v>37.398992800245097</v>
+      </c>
       <c r="N9" s="5"/>
       <c r="O9" s="5">
         <v>37.398992800245097</v>
@@ -1183,7 +1187,9 @@
       <c r="U9" s="5">
         <v>37.398992800245097</v>
       </c>
-      <c r="V9" s="4"/>
+      <c r="V9" s="4">
+        <v>4.1464100713315215</v>
+      </c>
       <c r="W9" s="5"/>
       <c r="X9" s="5">
         <v>5.7623825764728096</v>
@@ -1263,7 +1269,9 @@
       </c>
       <c r="BD9" s="5"/>
       <c r="BE9" s="5"/>
-      <c r="BF9" s="4"/>
+      <c r="BF9" s="4">
+        <v>0.36800089384767509</v>
+      </c>
       <c r="BG9" s="5"/>
       <c r="BH9" s="1">
         <v>0.68907103786578761</v>
@@ -1291,7 +1299,9 @@
       <c r="C10" s="2">
         <v>4</v>
       </c>
-      <c r="D10" s="7"/>
+      <c r="D10" s="7">
+        <v>2.109898930102323</v>
+      </c>
       <c r="E10" s="8"/>
       <c r="F10" s="8">
         <v>2.1192762586805558</v>
@@ -1308,7 +1318,9 @@
       <c r="L10" s="9">
         <v>2.2452603093731609</v>
       </c>
-      <c r="M10" s="7"/>
+      <c r="M10" s="7">
+        <v>68.119594029017861</v>
+      </c>
       <c r="N10" s="8"/>
       <c r="O10" s="8">
         <v>68.119594029017861</v>
@@ -1325,7 +1337,9 @@
       <c r="U10" s="8">
         <v>68.119594029017861</v>
       </c>
-      <c r="V10" s="7"/>
+      <c r="V10" s="7">
+        <v>12.975160767431973</v>
+      </c>
       <c r="W10" s="8"/>
       <c r="X10" s="8">
         <v>17.261073600113122</v>
@@ -1405,7 +1419,9 @@
       </c>
       <c r="BD10" s="8"/>
       <c r="BE10" s="8"/>
-      <c r="BF10" s="7"/>
+      <c r="BF10" s="7">
+        <v>0.73218757497600762</v>
+      </c>
       <c r="BG10" s="8"/>
       <c r="BH10" s="1">
         <v>1.3427304701249561</v>
@@ -1433,7 +1449,9 @@
       <c r="C11" s="2">
         <v>8</v>
       </c>
-      <c r="D11" s="7"/>
+      <c r="D11" s="7">
+        <v>4.1645166655294759</v>
+      </c>
       <c r="E11" s="8"/>
       <c r="F11" s="8">
         <v>4.1690680498633874</v>
@@ -1450,7 +1468,9 @@
       <c r="L11" s="9">
         <v>4.427971289175856</v>
       </c>
-      <c r="M11" s="7"/>
+      <c r="M11" s="7">
+        <v>149.59597120098039</v>
+      </c>
       <c r="N11" s="8"/>
       <c r="O11" s="8">
         <v>149.59597120098039</v>
@@ -1467,7 +1487,9 @@
       <c r="U11" s="8">
         <v>149.59597120098039</v>
       </c>
-      <c r="V11" s="7"/>
+      <c r="V11" s="7">
+        <v>15.927754762526096</v>
+      </c>
       <c r="W11" s="8"/>
       <c r="X11" s="8">
         <v>21.798270089285715</v>
@@ -1547,7 +1569,9 @@
       </c>
       <c r="BD11" s="8"/>
       <c r="BE11" s="8"/>
-      <c r="BF11" s="7"/>
+      <c r="BF11" s="7">
+        <v>1.459054222843756</v>
+      </c>
       <c r="BG11" s="8"/>
       <c r="BH11" s="1">
         <v>2.7025839643110166</v>
@@ -1575,7 +1599,9 @@
       <c r="C12" s="2">
         <v>16</v>
       </c>
-      <c r="D12" s="7"/>
+      <c r="D12" s="7">
+        <v>6.8241453767889091</v>
+      </c>
       <c r="E12" s="8"/>
       <c r="F12" s="8">
         <v>7.4505805969238272</v>
@@ -1592,7 +1618,9 @@
       <c r="L12" s="9">
         <v>7.6677331972361813</v>
       </c>
-      <c r="M12" s="7"/>
+      <c r="M12" s="7">
+        <v>282.57016782407408</v>
+      </c>
       <c r="N12" s="8"/>
       <c r="O12" s="8">
         <v>282.57016782407408</v>
@@ -1609,7 +1637,9 @@
       <c r="U12" s="8">
         <v>282.57016782407408</v>
       </c>
-      <c r="V12" s="7"/>
+      <c r="V12" s="7">
+        <v>17.261073600113122</v>
+      </c>
       <c r="W12" s="8"/>
       <c r="X12" s="8">
         <v>25.096692537006579</v>
@@ -1689,7 +1719,9 @@
       </c>
       <c r="BD12" s="8"/>
       <c r="BE12" s="8"/>
-      <c r="BF12" s="7"/>
+      <c r="BF12" s="7">
+        <v>2.9036706113225503</v>
+      </c>
       <c r="BG12" s="8"/>
       <c r="BH12" s="1">
         <v>5.3502065436535764</v>
@@ -1717,7 +1749,9 @@
       <c r="C13" s="2">
         <v>32</v>
       </c>
-      <c r="D13" s="7"/>
+      <c r="D13" s="7">
+        <v>10.914727512517883</v>
+      </c>
       <c r="E13" s="8"/>
       <c r="F13" s="8">
         <v>11.972372744213416</v>
@@ -1734,7 +1768,9 @@
       <c r="L13" s="9">
         <v>12.57938092539159</v>
       </c>
-      <c r="M13" s="7"/>
+      <c r="M13" s="7">
+        <v>469.50120192307691</v>
+      </c>
       <c r="N13" s="8"/>
       <c r="O13" s="8">
         <v>469.50120192307691</v>
@@ -1751,7 +1787,9 @@
       <c r="U13" s="8">
         <v>469.50120192307691</v>
       </c>
-      <c r="V13" s="7"/>
+      <c r="V13" s="7">
+        <v>31.855509525052192</v>
+      </c>
       <c r="W13" s="8"/>
       <c r="X13" s="8">
         <v>44.812890051395009</v>
@@ -1831,7 +1869,9 @@
       </c>
       <c r="BD13" s="8"/>
       <c r="BE13" s="8"/>
-      <c r="BF13" s="7"/>
+      <c r="BF13" s="7">
+        <v>5.6378308008498061</v>
+      </c>
       <c r="BG13" s="8"/>
       <c r="BH13" s="1">
         <v>10.387194732811436</v>
@@ -1859,7 +1899,9 @@
       <c r="C14" s="2">
         <v>64</v>
       </c>
-      <c r="D14" s="7"/>
+      <c r="D14" s="7">
+        <v>13.176847204231434</v>
+      </c>
       <c r="E14" s="8"/>
       <c r="F14" s="8">
         <v>14.594728897656625</v>
@@ -1876,7 +1918,9 @@
       <c r="L14" s="9">
         <v>16.367700791096809</v>
       </c>
-      <c r="M14" s="7"/>
+      <c r="M14" s="7">
+        <v>709.71111918604652</v>
+      </c>
       <c r="N14" s="8"/>
       <c r="O14" s="8">
         <v>709.71111918604652</v>
@@ -1893,7 +1937,9 @@
       <c r="U14" s="8">
         <v>709.71111918604652</v>
       </c>
-      <c r="V14" s="7"/>
+      <c r="V14" s="7">
+        <v>33.11728499728703</v>
+      </c>
       <c r="W14" s="8"/>
       <c r="X14" s="8">
         <v>50.193385074013158</v>
@@ -1973,7 +2019,9 @@
       </c>
       <c r="BD14" s="8"/>
       <c r="BE14" s="8"/>
-      <c r="BF14" s="7"/>
+      <c r="BF14" s="7">
+        <v>10.887469898323225</v>
+      </c>
       <c r="BG14" s="8"/>
       <c r="BH14" s="1">
         <v>20.379017111853088</v>
@@ -2001,7 +2049,9 @@
       <c r="C15" s="2">
         <v>128</v>
       </c>
-      <c r="D15" s="7"/>
+      <c r="D15" s="7">
+        <v>17.173651167698367</v>
+      </c>
       <c r="E15" s="8"/>
       <c r="F15" s="8">
         <v>19.852059277931371</v>
@@ -2018,7 +2068,9 @@
       <c r="L15" s="9">
         <v>22.92400234741784</v>
       </c>
-      <c r="M15" s="7"/>
+      <c r="M15" s="7">
+        <v>859.65008802816897</v>
+      </c>
       <c r="N15" s="8"/>
       <c r="O15" s="8">
         <v>871.93080357142856</v>
@@ -2035,7 +2087,9 @@
       <c r="U15" s="8">
         <v>878.2036870503598</v>
       </c>
-      <c r="V15" s="7"/>
+      <c r="V15" s="7">
+        <v>33.965028519755151</v>
+      </c>
       <c r="W15" s="8"/>
       <c r="X15" s="8">
         <v>51.746635226791007</v>
@@ -2115,7 +2169,9 @@
       </c>
       <c r="BD15" s="8"/>
       <c r="BE15" s="8"/>
-      <c r="BF15" s="7"/>
+      <c r="BF15" s="7">
+        <v>20.602584388185655</v>
+      </c>
       <c r="BG15" s="8"/>
       <c r="BH15" s="1">
         <v>36.823623680241326</v>
@@ -2143,7 +2199,9 @@
       <c r="C16" s="2">
         <v>256</v>
       </c>
-      <c r="D16" s="7"/>
+      <c r="D16" s="7">
+        <v>20.307821078023625</v>
+      </c>
       <c r="E16" s="8"/>
       <c r="F16" s="8">
         <v>23.622701983551039</v>
@@ -2160,7 +2218,9 @@
       <c r="L16" s="9">
         <v>28.66509627803217</v>
       </c>
-      <c r="M16" s="7"/>
+      <c r="M16" s="7">
+        <v>168.14092630853995</v>
+      </c>
       <c r="N16" s="8"/>
       <c r="O16" s="8">
         <v>305.55772841051316</v>
@@ -2177,7 +2237,9 @@
       <c r="U16" s="8">
         <v>627.61086118251933</v>
       </c>
-      <c r="V16" s="7"/>
+      <c r="V16" s="7">
+        <v>34.226920650497689</v>
+      </c>
       <c r="W16" s="8"/>
       <c r="X16" s="8">
         <v>52.571194013781223</v>
@@ -2257,7 +2319,9 @@
       </c>
       <c r="BD16" s="8"/>
       <c r="BE16" s="8"/>
-      <c r="BF16" s="7"/>
+      <c r="BF16" s="7">
+        <v>30.181805538385461</v>
+      </c>
       <c r="BG16" s="8"/>
       <c r="BH16" s="1">
         <v>65.138907417289218</v>
@@ -2285,7 +2349,9 @@
       <c r="C17" s="2">
         <v>512</v>
       </c>
-      <c r="D17" s="7"/>
+      <c r="D17" s="7">
+        <v>22.290858251540744</v>
+      </c>
       <c r="E17" s="8"/>
       <c r="F17" s="8">
         <v>26.362231400496707</v>
@@ -2302,7 +2368,9 @@
       <c r="L17" s="9">
         <v>32.763956921425219</v>
       </c>
-      <c r="M17" s="7"/>
+      <c r="M17" s="7">
+        <v>121.70519690927219</v>
+      </c>
       <c r="N17" s="8"/>
       <c r="O17" s="8">
         <v>235.2029142581888</v>
@@ -2319,7 +2387,9 @@
       <c r="U17" s="8">
         <v>537.75468061674007</v>
       </c>
-      <c r="V17" s="7"/>
+      <c r="V17" s="7">
+        <v>34.095471684938204</v>
+      </c>
       <c r="W17" s="8"/>
       <c r="X17" s="8">
         <v>52.981906467013893</v>
@@ -2399,7 +2469,9 @@
       </c>
       <c r="BD17" s="8"/>
       <c r="BE17" s="8"/>
-      <c r="BF17" s="7"/>
+      <c r="BF17" s="7">
+        <v>50.541481213124939</v>
+      </c>
       <c r="BG17" s="8"/>
       <c r="BH17" s="1">
         <v>105.23302801724139</v>
@@ -2427,7 +2499,9 @@
       <c r="C18" s="2">
         <v>1024</v>
       </c>
-      <c r="D18" s="7"/>
+      <c r="D18" s="7">
+        <v>23.323123402832511</v>
+      </c>
       <c r="E18" s="8"/>
       <c r="F18" s="8">
         <v>27.88266617176793</v>
@@ -2444,7 +2518,9 @@
       <c r="L18" s="9">
         <v>35.385263424885864</v>
       </c>
-      <c r="M18" s="7"/>
+      <c r="M18" s="7">
+        <v>106.86829722039835</v>
+      </c>
       <c r="N18" s="8"/>
       <c r="O18" s="8">
         <v>210.51142487605088</v>
@@ -2461,7 +2537,9 @@
       <c r="U18" s="8">
         <v>509.15667361835244</v>
       </c>
-      <c r="V18" s="7"/>
+      <c r="V18" s="7">
+        <v>34.516046371894106</v>
+      </c>
       <c r="W18" s="8"/>
       <c r="X18" s="8">
         <v>53.302903771628188</v>
@@ -2541,7 +2619,9 @@
       </c>
       <c r="BD18" s="8"/>
       <c r="BE18" s="8"/>
-      <c r="BF18" s="7"/>
+      <c r="BF18" s="7">
+        <v>76.311830897866685</v>
+      </c>
       <c r="BG18" s="8"/>
       <c r="BH18" s="1">
         <v>154.51938291139243</v>
@@ -2569,7 +2649,9 @@
       <c r="C19" s="2">
         <v>2048</v>
       </c>
-      <c r="D19" s="7"/>
+      <c r="D19" s="7">
+        <v>23.9667824230302</v>
+      </c>
       <c r="E19" s="8"/>
       <c r="F19" s="8">
         <v>28.709760399823608</v>
@@ -2586,7 +2668,9 @@
       <c r="L19" s="9">
         <v>36.838903768531445</v>
       </c>
-      <c r="M19" s="7"/>
+      <c r="M19" s="7">
+        <v>100.82726756491662</v>
+      </c>
       <c r="N19" s="8"/>
       <c r="O19" s="8">
         <v>200.15628202500511</v>
@@ -2603,7 +2687,9 @@
       <c r="U19" s="8">
         <v>491.22862173038232</v>
       </c>
-      <c r="V19" s="7"/>
+      <c r="V19" s="7">
+        <v>34.583274311211845</v>
+      </c>
       <c r="W19" s="8"/>
       <c r="X19" s="8">
         <v>53.409308430637971</v>
@@ -2683,7 +2769,9 @@
       </c>
       <c r="BD19" s="8"/>
       <c r="BE19" s="8"/>
-      <c r="BF19" s="7"/>
+      <c r="BF19" s="7">
+        <v>101.69348120379048</v>
+      </c>
       <c r="BG19" s="8"/>
       <c r="BH19" s="1">
         <v>199.78774549918168</v>
@@ -2711,7 +2799,9 @@
       <c r="C20" s="2">
         <v>4096</v>
       </c>
-      <c r="D20" s="7"/>
+      <c r="D20" s="7">
+        <v>24.312254932470282</v>
+      </c>
       <c r="E20" s="8"/>
       <c r="F20" s="8">
         <v>29.152424735435918</v>
@@ -2728,7 +2818,9 @@
       <c r="L20" s="9">
         <v>37.634279107856834</v>
       </c>
-      <c r="M20" s="7"/>
+      <c r="M20" s="7">
+        <v>98.038600542114239</v>
+      </c>
       <c r="N20" s="8"/>
       <c r="O20" s="8">
         <v>195.38088330915821</v>
@@ -2745,7 +2837,9 @@
       <c r="U20" s="8">
         <v>484.10583715454209</v>
       </c>
-      <c r="V20" s="7"/>
+      <c r="V20" s="7">
+        <v>34.54962763793317</v>
+      </c>
       <c r="W20" s="8"/>
       <c r="X20" s="8">
         <v>53.436341500116278</v>
@@ -2825,7 +2919,9 @@
       </c>
       <c r="BD20" s="8"/>
       <c r="BE20" s="8"/>
-      <c r="BF20" s="7"/>
+      <c r="BF20" s="7">
+        <v>122.20779627080465</v>
+      </c>
       <c r="BG20" s="8"/>
       <c r="BH20" s="1">
         <v>232.25221475711993</v>
@@ -2853,7 +2949,9 @@
       <c r="C21" s="2">
         <v>8192</v>
       </c>
-      <c r="D21" s="7"/>
+      <c r="D21" s="7">
+        <v>24.483227618020909</v>
+      </c>
       <c r="E21" s="8"/>
       <c r="F21" s="8">
         <v>29.363898097407333</v>
@@ -2870,7 +2968,9 @@
       <c r="L21" s="9">
         <v>38.047951376544439</v>
       </c>
-      <c r="M21" s="7"/>
+      <c r="M21" s="7">
+        <v>96.703718374015949</v>
+      </c>
       <c r="N21" s="8"/>
       <c r="O21" s="8">
         <v>193.08239829963918</v>
@@ -2887,7 +2987,9 @@
       <c r="U21" s="8">
         <v>480.47355473554734</v>
       </c>
-      <c r="V21" s="7"/>
+      <c r="V21" s="7">
+        <v>34.620054594441292</v>
+      </c>
       <c r="W21" s="8"/>
       <c r="X21" s="8">
         <v>53.435976005964314</v>
@@ -2967,7 +3069,9 @@
       </c>
       <c r="BD21" s="8"/>
       <c r="BE21" s="8"/>
-      <c r="BF21" s="7"/>
+      <c r="BF21" s="7">
+        <v>136.02333072168537</v>
+      </c>
       <c r="BG21" s="8"/>
       <c r="BH21" s="1">
         <v>254.71113719353156</v>
@@ -2995,7 +3099,9 @@
       <c r="C22" s="2">
         <v>16384</v>
       </c>
-      <c r="D22" s="7"/>
+      <c r="D22" s="7">
+        <v>24.265097549574566</v>
+      </c>
       <c r="E22" s="8"/>
       <c r="F22" s="8">
         <v>29.125688764287897</v>
@@ -3012,7 +3118,9 @@
       <c r="L22" s="9">
         <v>37.536545580777442</v>
       </c>
-      <c r="M22" s="7"/>
+      <c r="M22" s="7">
+        <v>96.040370761930518</v>
+      </c>
       <c r="N22" s="8"/>
       <c r="O22" s="8">
         <v>191.81899652577434</v>
@@ -3029,7 +3137,9 @@
       <c r="U22" s="8">
         <v>478.32608828751603</v>
       </c>
-      <c r="V22" s="7"/>
+      <c r="V22" s="7">
+        <v>34.562084563743539</v>
+      </c>
       <c r="W22" s="8"/>
       <c r="X22" s="8">
         <v>53.455902729073507</v>
@@ -3109,7 +3219,9 @@
       </c>
       <c r="BD22" s="8"/>
       <c r="BE22" s="8"/>
-      <c r="BF22" s="7"/>
+      <c r="BF22" s="7">
+        <v>141.03513015850092</v>
+      </c>
       <c r="BG22" s="8"/>
       <c r="BH22" s="1">
         <v>266.12958168687828</v>
@@ -3137,7 +3249,9 @@
       <c r="C23" s="2">
         <v>32768</v>
       </c>
-      <c r="D23" s="7"/>
+      <c r="D23" s="7">
+        <v>24.424003832810072</v>
+      </c>
       <c r="E23" s="8"/>
       <c r="F23" s="8">
         <v>29.353361875759667</v>
@@ -3154,7 +3268,9 @@
       <c r="L23" s="9">
         <v>37.995999781143041</v>
       </c>
-      <c r="M23" s="7"/>
+      <c r="M23" s="7">
+        <v>95.70652856342204</v>
+      </c>
       <c r="N23" s="8"/>
       <c r="O23" s="8">
         <v>191.24378840175271</v>
@@ -3171,7 +3287,9 @@
       <c r="U23" s="8">
         <v>477.58776152705826</v>
       </c>
-      <c r="V23" s="7"/>
+      <c r="V23" s="7">
+        <v>34.523329485132876</v>
+      </c>
       <c r="W23" s="8"/>
       <c r="X23" s="8">
         <v>53.396988238992961</v>
@@ -3251,7 +3369,9 @@
       </c>
       <c r="BD23" s="8"/>
       <c r="BE23" s="8"/>
-      <c r="BF23" s="7"/>
+      <c r="BF23" s="7">
+        <v>147.40844166871074</v>
+      </c>
       <c r="BG23" s="8"/>
       <c r="BH23" s="1">
         <v>267.17622516329811</v>
@@ -3279,7 +3399,9 @@
       <c r="C24" s="2">
         <v>65536</v>
       </c>
-      <c r="D24" s="7"/>
+      <c r="D24" s="7">
+        <v>24.426399740181271</v>
+      </c>
       <c r="E24" s="8"/>
       <c r="F24" s="8">
         <v>29.35773266237997</v>
@@ -3296,7 +3418,9 @@
       <c r="L24" s="9">
         <v>38.002353105704309</v>
       </c>
-      <c r="M24" s="7"/>
+      <c r="M24" s="7">
+        <v>95.563411292690091</v>
+      </c>
       <c r="N24" s="8"/>
       <c r="O24" s="8">
         <v>191.00416236270621</v>
@@ -3313,7 +3437,9 @@
       <c r="U24" s="8">
         <v>477.08102744170066</v>
       </c>
-      <c r="V24" s="7"/>
+      <c r="V24" s="7">
+        <v>34.574034070636131</v>
+      </c>
       <c r="W24" s="8"/>
       <c r="X24" s="8">
         <v>53.415470658668305</v>
@@ -3393,7 +3519,9 @@
       </c>
       <c r="BD24" s="8"/>
       <c r="BE24" s="8"/>
-      <c r="BF24" s="7"/>
+      <c r="BF24" s="7">
+        <v>148.88006460203763</v>
+      </c>
       <c r="BG24" s="8"/>
       <c r="BH24" s="1">
         <v>242.9061682620744</v>
@@ -3421,7 +3549,9 @@
       <c r="C25" s="2">
         <v>131072</v>
       </c>
-      <c r="D25" s="7"/>
+      <c r="D25" s="7">
+        <v>24.428361679678513</v>
+      </c>
       <c r="E25" s="8"/>
       <c r="F25" s="8">
         <v>29.358704891230694</v>
@@ -3438,7 +3568,9 @@
       <c r="L25" s="9">
         <v>38.006767028855954</v>
       </c>
-      <c r="M25" s="7"/>
+      <c r="M25" s="7">
+        <v>95.490481126879345</v>
+      </c>
       <c r="N25" s="8"/>
       <c r="O25" s="8">
         <v>190.86125760772973</v>
@@ -3455,7 +3587,9 @@
       <c r="U25" s="8">
         <v>476.96270151674139</v>
       </c>
-      <c r="V25" s="7"/>
+      <c r="V25" s="7">
+        <v>34.571911234820163</v>
+      </c>
       <c r="W25" s="8"/>
       <c r="X25" s="8">
         <v>53.423871837413643</v>
@@ -3535,7 +3669,9 @@
       </c>
       <c r="BD25" s="8"/>
       <c r="BE25" s="8"/>
-      <c r="BF25" s="7"/>
+      <c r="BF25" s="7">
+        <v>148.59830193748411</v>
+      </c>
       <c r="BG25" s="8"/>
       <c r="BH25" s="1">
         <v>225.9062001312063</v>
@@ -3563,7 +3699,9 @@
       <c r="C26" s="2">
         <v>262144</v>
       </c>
-      <c r="D26" s="7"/>
+      <c r="D26" s="7">
+        <v>24.429536130013599</v>
+      </c>
       <c r="E26" s="8"/>
       <c r="F26" s="8">
         <v>29.358566982510045</v>
@@ -3580,7 +3718,9 @@
       <c r="L26" s="9">
         <v>38.008766341869084</v>
       </c>
-      <c r="M26" s="7"/>
+      <c r="M26" s="7">
+        <v>95.452709291519454</v>
+      </c>
       <c r="N26" s="8"/>
       <c r="O26" s="8">
         <v>190.79949567877301</v>
@@ -3597,7 +3737,9 @@
       <c r="U26" s="8">
         <v>476.90356056198317</v>
       </c>
-      <c r="V26" s="7"/>
+      <c r="V26" s="7">
+        <v>34.548658399587296</v>
+      </c>
       <c r="W26" s="8"/>
       <c r="X26" s="8">
         <v>52.953312123766715</v>
@@ -3677,7 +3819,9 @@
       </c>
       <c r="BD26" s="8"/>
       <c r="BE26" s="8"/>
-      <c r="BF26" s="7"/>
+      <c r="BF26" s="7">
+        <v>147.23585299030128</v>
+      </c>
       <c r="BG26" s="8"/>
       <c r="BH26" s="1">
         <v>154.55816765728147</v>
@@ -3705,7 +3849,9 @@
       <c r="C27" s="2">
         <v>524288</v>
       </c>
-      <c r="D27" s="7"/>
+      <c r="D27" s="7">
+        <v>24.430725017922381</v>
+      </c>
       <c r="E27" s="8"/>
       <c r="F27" s="8">
         <v>29.359199649427669</v>
@@ -3722,7 +3868,9 @@
       <c r="L27" s="9">
         <v>38.009858540990059</v>
       </c>
-      <c r="M27" s="7"/>
+      <c r="M27" s="7">
+        <v>95.433452058909921</v>
+      </c>
       <c r="N27" s="8"/>
       <c r="O27" s="8">
         <v>190.76666451736227</v>
@@ -3739,7 +3887,9 @@
       <c r="U27" s="8">
         <v>476.84625332361838</v>
       </c>
-      <c r="V27" s="7"/>
+      <c r="V27" s="7">
+        <v>34.569544867051754</v>
+      </c>
       <c r="W27" s="8"/>
       <c r="X27" s="8">
         <v>53.408794975813294</v>
@@ -3819,7 +3969,9 @@
       </c>
       <c r="BD27" s="8"/>
       <c r="BE27" s="8"/>
-      <c r="BF27" s="7"/>
+      <c r="BF27" s="7">
+        <v>133.76709543479657</v>
+      </c>
       <c r="BG27" s="8"/>
       <c r="BH27" s="1">
         <v>196.00994319239825</v>
@@ -3847,7 +3999,9 @@
       <c r="C28" s="2">
         <v>1048576</v>
       </c>
-      <c r="D28" s="7"/>
+      <c r="D28" s="7">
+        <v>24.431671078171355</v>
+      </c>
       <c r="E28" s="8"/>
       <c r="F28" s="8">
         <v>29.359222922436427</v>
@@ -3864,7 +4018,9 @@
       <c r="L28" s="9">
         <v>38.010572260568551</v>
       </c>
-      <c r="M28" s="7"/>
+      <c r="M28" s="7">
+        <v>95.422469625119462</v>
+      </c>
       <c r="N28" s="8"/>
       <c r="O28" s="8">
         <v>190.74061146099297</v>
@@ -3881,7 +4037,9 @@
       <c r="U28" s="8">
         <v>472.02073492684383</v>
       </c>
-      <c r="V28" s="7"/>
+      <c r="V28" s="7">
+        <v>34.55533793755567</v>
+      </c>
       <c r="W28" s="8"/>
       <c r="X28" s="8">
         <v>53.38505847238762</v>
@@ -3961,7 +4119,9 @@
       </c>
       <c r="BD28" s="8"/>
       <c r="BE28" s="8"/>
-      <c r="BF28" s="7"/>
+      <c r="BF28" s="7">
+        <v>126.23621547865554</v>
+      </c>
       <c r="BG28" s="8"/>
       <c r="BH28" s="1">
         <v>193.65996022224417</v>
@@ -3989,7 +4149,9 @@
       <c r="C29" s="2">
         <v>2097152</v>
       </c>
-      <c r="D29" s="10"/>
+      <c r="D29" s="10">
+        <v>24.431984756591529</v>
+      </c>
       <c r="E29" s="11"/>
       <c r="F29" s="11">
         <v>29.359232404043169</v>
@@ -4006,7 +4168,9 @@
       <c r="L29" s="12">
         <v>38.01086628037617</v>
       </c>
-      <c r="M29" s="10"/>
+      <c r="M29" s="10">
+        <v>95.418445186969578</v>
+      </c>
       <c r="N29" s="11"/>
       <c r="O29" s="11">
         <v>190.73540897963233</v>
@@ -4023,7 +4187,9 @@
       <c r="U29" s="11">
         <v>469.02577249717297</v>
       </c>
-      <c r="V29" s="7"/>
+      <c r="V29" s="7">
+        <v>34.49964679261614</v>
+      </c>
       <c r="W29" s="8"/>
       <c r="X29" s="8">
         <v>53.391609919616535</v>
@@ -4103,7 +4269,9 @@
       </c>
       <c r="BD29" s="11"/>
       <c r="BE29" s="11"/>
-      <c r="BF29" s="7"/>
+      <c r="BF29" s="7">
+        <v>129.34223716671173</v>
+      </c>
       <c r="BG29" s="8"/>
       <c r="BH29" s="11">
         <v>211.96250680002217</v>
@@ -4135,7 +4303,9 @@
       <c r="C30" s="15">
         <v>2</v>
       </c>
-      <c r="D30" s="4"/>
+      <c r="D30" s="4">
+        <v>0.9686889958417978</v>
+      </c>
       <c r="E30" s="5"/>
       <c r="F30" s="5">
         <v>0.99652488652690707</v>
@@ -4152,7 +4322,9 @@
       <c r="L30" s="6">
         <v>1.0243547974288401</v>
       </c>
-      <c r="M30" s="4"/>
+      <c r="M30" s="4">
+        <v>34.059797014508931</v>
+      </c>
       <c r="N30" s="5"/>
       <c r="O30" s="5">
         <v>34.059797014508931</v>
@@ -4169,7 +4341,9 @@
       <c r="U30" s="5">
         <v>34.059797014508931</v>
       </c>
-      <c r="V30" s="4"/>
+      <c r="V30" s="4">
+        <v>4.1464100713315215</v>
+      </c>
       <c r="W30" s="5"/>
       <c r="X30" s="5">
         <v>6.0937656000399363</v>
@@ -4249,7 +4423,9 @@
       </c>
       <c r="BD30" s="5"/>
       <c r="BE30" s="5"/>
-      <c r="BF30" s="4"/>
+      <c r="BF30" s="4">
+        <v>0.36630471150614557</v>
+      </c>
       <c r="BG30" s="5"/>
       <c r="BH30" s="1">
         <v>0.68363750280017921</v>
@@ -4277,7 +4453,9 @@
       <c r="C31" s="2">
         <v>4</v>
       </c>
-      <c r="D31" s="7"/>
+      <c r="D31" s="7">
+        <v>2.024786234408174</v>
+      </c>
       <c r="E31" s="8"/>
       <c r="F31" s="8">
         <v>2.0936867539105379</v>
@@ -4294,7 +4472,9 @@
       <c r="L31" s="9">
         <v>2.0653477345018949</v>
       </c>
-      <c r="M31" s="7"/>
+      <c r="M31" s="7">
+        <v>14.728560871138997</v>
+      </c>
       <c r="N31" s="8"/>
       <c r="O31" s="8">
         <v>19.76527080634715</v>
@@ -4311,7 +4491,9 @@
       <c r="U31" s="8">
         <v>29.119826455152673</v>
       </c>
-      <c r="V31" s="7"/>
+      <c r="V31" s="7">
+        <v>13.821366904438406</v>
+      </c>
       <c r="W31" s="8"/>
       <c r="X31" s="8">
         <v>18.884639928836634</v>
@@ -4391,7 +4573,9 @@
       </c>
       <c r="BD31" s="8"/>
       <c r="BE31" s="8"/>
-      <c r="BF31" s="7"/>
+      <c r="BF31" s="7">
+        <v>0.74578636669110454</v>
+      </c>
       <c r="BG31" s="8"/>
       <c r="BH31" s="1">
         <v>1.3998889048165137</v>
@@ -4419,7 +4603,9 @@
       <c r="C32" s="2">
         <v>8</v>
       </c>
-      <c r="D32" s="7"/>
+      <c r="D32" s="7">
+        <v>4.0091405839464</v>
+      </c>
       <c r="E32" s="8"/>
       <c r="F32" s="8">
         <v>4.077709530331374</v>
@@ -4436,7 +4622,9 @@
       <c r="L32" s="9">
         <v>4.166791114827963</v>
       </c>
-      <c r="M32" s="7"/>
+      <c r="M32" s="7">
+        <v>136.23918805803572</v>
+      </c>
       <c r="N32" s="8"/>
       <c r="O32" s="8">
         <v>136.23918805803572</v>
@@ -4453,7 +4641,9 @@
       <c r="U32" s="8">
         <v>136.23918805803572</v>
       </c>
-      <c r="V32" s="7"/>
+      <c r="V32" s="7">
+        <v>15.927754762526096</v>
+      </c>
       <c r="W32" s="8"/>
       <c r="X32" s="8">
         <v>23.049530305891238</v>
@@ -4533,7 +4723,9 @@
       </c>
       <c r="BD32" s="8"/>
       <c r="BE32" s="8"/>
-      <c r="BF32" s="7"/>
+      <c r="BF32" s="7">
+        <v>1.4626906693347395</v>
+      </c>
       <c r="BG32" s="8"/>
       <c r="BH32" s="1">
         <v>2.6968520789148109</v>
@@ -4561,7 +4753,9 @@
       <c r="C33" s="2">
         <v>16</v>
       </c>
-      <c r="D33" s="7"/>
+      <c r="D33" s="7">
+        <v>7.0058719295224972</v>
+      </c>
       <c r="E33" s="8"/>
       <c r="F33" s="8">
         <v>7.3678363411395456</v>
@@ -4578,7 +4772,9 @@
       <c r="L33" s="9">
         <v>7.8613029688304996</v>
       </c>
-      <c r="M33" s="7"/>
+      <c r="M33" s="7">
+        <v>52.981906467013893</v>
+      </c>
       <c r="N33" s="8"/>
       <c r="O33" s="8">
         <v>73.713956823671495</v>
@@ -4595,7 +4791,9 @@
       <c r="U33" s="8">
         <v>108.99135044642857</v>
       </c>
-      <c r="V33" s="7"/>
+      <c r="V33" s="7">
+        <v>17.261073600113122</v>
+      </c>
       <c r="W33" s="8"/>
       <c r="X33" s="8">
         <v>26.722923051663749</v>
@@ -4675,7 +4873,9 @@
       </c>
       <c r="BD33" s="8"/>
       <c r="BE33" s="8"/>
-      <c r="BF33" s="7"/>
+      <c r="BF33" s="7">
+        <v>2.7281940036652963</v>
+      </c>
       <c r="BG33" s="8"/>
       <c r="BH33" s="1">
         <v>4.8317888101646611</v>
@@ -4703,7 +4903,9 @@
       <c r="C34" s="2">
         <v>32</v>
       </c>
-      <c r="D34" s="7"/>
+      <c r="D34" s="7">
+        <v>10.930364657951289</v>
+      </c>
       <c r="E34" s="8"/>
       <c r="F34" s="8">
         <v>12.340306560857259</v>
@@ -4720,7 +4922,9 @@
       <c r="L34" s="9">
         <v>13.734283584608461</v>
       </c>
-      <c r="M34" s="7"/>
+      <c r="M34" s="7">
+        <v>57.58033608490566</v>
+      </c>
       <c r="N34" s="8"/>
       <c r="O34" s="8">
         <v>78.451357647814916</v>
@@ -4737,7 +4941,9 @@
       <c r="U34" s="8">
         <v>123.05475050403226</v>
       </c>
-      <c r="V34" s="7"/>
+      <c r="V34" s="7">
+        <v>42.503590703342617</v>
+      </c>
       <c r="W34" s="8"/>
       <c r="X34" s="8">
         <v>69.044294400452486</v>
@@ -4817,7 +5023,9 @@
       </c>
       <c r="BD34" s="8"/>
       <c r="BE34" s="8"/>
-      <c r="BF34" s="7"/>
+      <c r="BF34" s="7">
+        <v>5.4340416889245011</v>
+      </c>
       <c r="BG34" s="8"/>
       <c r="BH34" s="1">
         <v>10.121916459369817</v>
@@ -4845,7 +5053,9 @@
       <c r="C35" s="2">
         <v>64</v>
       </c>
-      <c r="D35" s="7"/>
+      <c r="D35" s="7">
+        <v>13.367314115199299</v>
+      </c>
       <c r="E35" s="8"/>
       <c r="F35" s="8">
         <v>15.886297826652786</v>
@@ -4862,7 +5072,9 @@
       <c r="L35" s="9">
         <v>18.214012608176663</v>
       </c>
-      <c r="M35" s="7"/>
+      <c r="M35" s="7">
+        <v>51.075444560669453</v>
+      </c>
       <c r="N35" s="8"/>
       <c r="O35" s="8">
         <v>108.99135044642857</v>
@@ -4879,7 +5091,9 @@
       <c r="U35" s="8">
         <v>172.41569562146893</v>
       </c>
-      <c r="V35" s="7"/>
+      <c r="V35" s="7">
+        <v>44.780011922230379</v>
+      </c>
       <c r="W35" s="8"/>
       <c r="X35" s="8">
         <v>78.856791020671835</v>
@@ -4959,7 +5173,9 @@
       </c>
       <c r="BD35" s="8"/>
       <c r="BE35" s="8"/>
-      <c r="BF35" s="7"/>
+      <c r="BF35" s="7">
+        <v>9.7985481216888743</v>
+      </c>
       <c r="BG35" s="8"/>
       <c r="BH35" s="1">
         <v>17.830895778556823</v>
@@ -4987,7 +5203,9 @@
       <c r="C36" s="2">
         <v>128</v>
       </c>
-      <c r="D36" s="7"/>
+      <c r="D36" s="7">
+        <v>17.596988972178174</v>
+      </c>
       <c r="E36" s="8"/>
       <c r="F36" s="8">
         <v>21.340963723776223</v>
@@ -5004,7 +5222,9 @@
       <c r="L36" s="9">
         <v>26.427865880060619</v>
       </c>
-      <c r="M36" s="7"/>
+      <c r="M36" s="7">
+        <v>48.906375200320518</v>
+      </c>
       <c r="N36" s="8"/>
       <c r="O36" s="8">
         <v>98.682548504446245</v>
@@ -5021,7 +5241,9 @@
       <c r="U36" s="8">
         <v>184.39624244712991</v>
       </c>
-      <c r="V36" s="7"/>
+      <c r="V36" s="7">
+        <v>46.326494307400374</v>
+      </c>
       <c r="W36" s="8"/>
       <c r="X36" s="8">
         <v>82.815680122116689</v>
@@ -5101,7 +5323,9 @@
       </c>
       <c r="BD36" s="8"/>
       <c r="BE36" s="8"/>
-      <c r="BF36" s="7"/>
+      <c r="BF36" s="7">
+        <v>16.198289875265392</v>
+      </c>
       <c r="BG36" s="8"/>
       <c r="BH36" s="1">
         <v>29.217403662039256</v>
@@ -5129,7 +5353,9 @@
       <c r="C37" s="2">
         <v>256</v>
       </c>
-      <c r="D37" s="7"/>
+      <c r="D37" s="7">
+        <v>20.838223369750768</v>
+      </c>
       <c r="E37" s="8"/>
       <c r="F37" s="8">
         <v>26.308257004310349</v>
@@ -5146,7 +5372,9 @@
       <c r="L37" s="9">
         <v>34.222122932436221</v>
       </c>
-      <c r="M37" s="7"/>
+      <c r="M37" s="7">
+        <v>58.532875809158469</v>
+      </c>
       <c r="N37" s="8"/>
       <c r="O37" s="8">
         <v>108.21836214539006</v>
@@ -5163,7 +5391,9 @@
       <c r="U37" s="8">
         <v>191.63314364207221</v>
       </c>
-      <c r="V37" s="7"/>
+      <c r="V37" s="7">
+        <v>47.479701478024111</v>
+      </c>
       <c r="W37" s="8"/>
       <c r="X37" s="8">
         <v>84.918478260869563</v>
@@ -5243,7 +5473,9 @@
       </c>
       <c r="BD37" s="8"/>
       <c r="BE37" s="8"/>
-      <c r="BF37" s="7"/>
+      <c r="BF37" s="7">
+        <v>21.115777979588305</v>
+      </c>
       <c r="BG37" s="8"/>
       <c r="BH37" s="1">
         <v>42.400247481764502</v>
@@ -5271,7 +5503,9 @@
       <c r="C38" s="2">
         <v>512</v>
       </c>
-      <c r="D38" s="7"/>
+      <c r="D38" s="7">
+        <v>22.956335213916311</v>
+      </c>
       <c r="E38" s="8"/>
       <c r="F38" s="8">
         <v>29.673731388635673</v>
@@ -5288,7 +5522,9 @@
       <c r="L38" s="9">
         <v>40.088772577996714</v>
       </c>
-      <c r="M38" s="7"/>
+      <c r="M38" s="7">
+        <v>64.818963228461442</v>
+      </c>
       <c r="N38" s="8"/>
       <c r="O38" s="8">
         <v>113.65950884543761</v>
@@ -5305,7 +5541,9 @@
       <c r="U38" s="8">
         <v>195.46887510008006</v>
       </c>
-      <c r="V38" s="7"/>
+      <c r="V38" s="7">
+        <v>47.908285910518053</v>
+      </c>
       <c r="W38" s="8"/>
       <c r="X38" s="8">
         <v>86.29926652527395</v>
@@ -5385,7 +5623,9 @@
       </c>
       <c r="BD38" s="8"/>
       <c r="BE38" s="8"/>
-      <c r="BF38" s="7"/>
+      <c r="BF38" s="7">
+        <v>29.977974582514733</v>
+      </c>
       <c r="BG38" s="8"/>
       <c r="BH38" s="1">
         <v>55.49281168314581</v>
@@ -5413,7 +5653,9 @@
       <c r="C39" s="2">
         <v>1024</v>
       </c>
-      <c r="D39" s="7"/>
+      <c r="D39" s="7">
+        <v>24.086486286503554</v>
+      </c>
       <c r="E39" s="8"/>
       <c r="F39" s="8">
         <v>31.594762043417777</v>
@@ -5430,7 +5672,9 @@
       <c r="L39" s="9">
         <v>43.837253669704175</v>
       </c>
-      <c r="M39" s="7"/>
+      <c r="M39" s="7">
+        <v>71.334002921840764</v>
+      </c>
       <c r="N39" s="8"/>
       <c r="O39" s="8">
         <v>142.08678888403898</v>
@@ -5447,7 +5691,9 @@
       <c r="U39" s="8">
         <v>264.43609531546167</v>
       </c>
-      <c r="V39" s="7"/>
+      <c r="V39" s="7">
+        <v>47.990687503071399</v>
+      </c>
       <c r="W39" s="8"/>
       <c r="X39" s="8">
         <v>86.859601529840788</v>
@@ -5527,7 +5773,9 @@
       </c>
       <c r="BD39" s="8"/>
       <c r="BE39" s="8"/>
-      <c r="BF39" s="7"/>
+      <c r="BF39" s="7">
+        <v>37.32038445370123</v>
+      </c>
       <c r="BG39" s="8"/>
       <c r="BH39" s="1">
         <v>64.591738871618489</v>
@@ -5555,7 +5803,9 @@
       <c r="C40" s="2">
         <v>2048</v>
       </c>
-      <c r="D40" s="7"/>
+      <c r="D40" s="7">
+        <v>24.707151079682738</v>
+      </c>
       <c r="E40" s="8"/>
       <c r="F40" s="8">
         <v>32.738145124792574</v>
@@ -5572,7 +5822,9 @@
       <c r="L40" s="9">
         <v>46.053407215279414</v>
       </c>
-      <c r="M40" s="7"/>
+      <c r="M40" s="7">
+        <v>73.636140853566587</v>
+      </c>
       <c r="N40" s="8"/>
       <c r="O40" s="8">
         <v>145.95165147212674</v>
@@ -5589,7 +5841,9 @@
       <c r="U40" s="8">
         <v>269.88047533508359</v>
       </c>
-      <c r="V40" s="7"/>
+      <c r="V40" s="7">
+        <v>48.165844636251535</v>
+      </c>
       <c r="W40" s="8"/>
       <c r="X40" s="8">
         <v>87.072578128482903</v>
@@ -5669,7 +5923,9 @@
       </c>
       <c r="BD40" s="8"/>
       <c r="BE40" s="8"/>
-      <c r="BF40" s="7"/>
+      <c r="BF40" s="7">
+        <v>42.516544037615915</v>
+      </c>
       <c r="BG40" s="8"/>
       <c r="BH40" s="1">
         <v>73.000373761913664</v>
@@ -5697,7 +5953,9 @@
       <c r="C41" s="2">
         <v>4096</v>
       </c>
-      <c r="D41" s="7"/>
+      <c r="D41" s="7">
+        <v>25.059179758918663</v>
+      </c>
       <c r="E41" s="8"/>
       <c r="F41" s="8">
         <v>33.31471262995403</v>
@@ -5714,7 +5972,9 @@
       <c r="L41" s="9">
         <v>47.223128906297219</v>
       </c>
-      <c r="M41" s="7"/>
+      <c r="M41" s="7">
+        <v>74.846713929871626</v>
+      </c>
       <c r="N41" s="8"/>
       <c r="O41" s="8">
         <v>148.00325843973781</v>
@@ -5731,7 +5991,9 @@
       <c r="U41" s="8">
         <v>272.63051367950862</v>
       </c>
-      <c r="V41" s="7"/>
+      <c r="V41" s="7">
+        <v>48.286113377339369</v>
+      </c>
       <c r="W41" s="8"/>
       <c r="X41" s="8">
         <v>87.212547443625809</v>
@@ -5811,7 +6073,9 @@
       </c>
       <c r="BD41" s="8"/>
       <c r="BE41" s="8"/>
-      <c r="BF41" s="7"/>
+      <c r="BF41" s="7">
+        <v>43.275835327483826</v>
+      </c>
       <c r="BG41" s="8"/>
       <c r="BH41" s="1">
         <v>76.624688597265546</v>
@@ -5839,7 +6103,9 @@
       <c r="C42" s="2">
         <v>8192</v>
       </c>
-      <c r="D42" s="7"/>
+      <c r="D42" s="7">
+        <v>25.233765604560649</v>
+      </c>
       <c r="E42" s="8"/>
       <c r="F42" s="8">
         <v>33.617911192774244</v>
@@ -5856,7 +6122,9 @@
       <c r="L42" s="9">
         <v>47.835537594905709</v>
       </c>
-      <c r="M42" s="7"/>
+      <c r="M42" s="7">
+        <v>75.611668150671676</v>
+      </c>
       <c r="N42" s="8"/>
       <c r="O42" s="8">
         <v>150.61402324998554</v>
@@ -5873,7 +6141,9 @@
       <c r="U42" s="8">
         <v>278.48078705353959</v>
       </c>
-      <c r="V42" s="7"/>
+      <c r="V42" s="7">
+        <v>48.280443716589936</v>
+      </c>
       <c r="W42" s="8"/>
       <c r="X42" s="8">
         <v>87.140562607357168</v>
@@ -5953,7 +6223,9 @@
       </c>
       <c r="BD42" s="8"/>
       <c r="BE42" s="8"/>
-      <c r="BF42" s="7"/>
+      <c r="BF42" s="7">
+        <v>47.43271384944174</v>
+      </c>
       <c r="BG42" s="8"/>
       <c r="BH42" s="1">
         <v>78.996329514545437</v>
@@ -5981,7 +6253,9 @@
       <c r="C43" s="2">
         <v>16384</v>
       </c>
-      <c r="D43" s="7"/>
+      <c r="D43" s="7">
+        <v>25.322056037507437</v>
+      </c>
       <c r="E43" s="8"/>
       <c r="F43" s="8">
         <v>33.769472828812006</v>
@@ -5998,7 +6272,9 @@
       <c r="L43" s="9">
         <v>48.148182386855623</v>
       </c>
-      <c r="M43" s="7"/>
+      <c r="M43" s="7">
+        <v>75.999299590454982</v>
+      </c>
       <c r="N43" s="8"/>
       <c r="O43" s="8">
         <v>151.5004605614001</v>
@@ -6015,7 +6291,9 @@
       <c r="U43" s="8">
         <v>281.35916735693451</v>
       </c>
-      <c r="V43" s="7"/>
+      <c r="V43" s="7">
+        <v>48.28029453297119</v>
+      </c>
       <c r="W43" s="8"/>
       <c r="X43" s="8">
         <v>87.23932888529076</v>
@@ -6095,7 +6373,9 @@
       </c>
       <c r="BD43" s="8"/>
       <c r="BE43" s="8"/>
-      <c r="BF43" s="7"/>
+      <c r="BF43" s="7">
+        <v>48.027417892326369</v>
+      </c>
       <c r="BG43" s="8"/>
       <c r="BH43" s="1">
         <v>80.182482500975013</v>
@@ -6123,7 +6403,9 @@
       <c r="C44" s="2">
         <v>32768</v>
       </c>
-      <c r="D44" s="7"/>
+      <c r="D44" s="7">
+        <v>25.329506483948389</v>
+      </c>
       <c r="E44" s="8"/>
       <c r="F44" s="8">
         <v>33.847050324335974</v>
@@ -6140,7 +6422,9 @@
       <c r="L44" s="9">
         <v>48.303951649676556</v>
       </c>
-      <c r="M44" s="7"/>
+      <c r="M44" s="7">
+        <v>76.204642996488488</v>
+      </c>
       <c r="N44" s="8"/>
       <c r="O44" s="8">
         <v>151.61071220648165</v>
@@ -6157,7 +6441,9 @@
       <c r="U44" s="8">
         <v>281.64825062638573</v>
       </c>
-      <c r="V44" s="7"/>
+      <c r="V44" s="7">
+        <v>48.221141382843456</v>
+      </c>
       <c r="W44" s="8"/>
       <c r="X44" s="8">
         <v>87.203299493802291</v>
@@ -6237,7 +6523,9 @@
       </c>
       <c r="BD44" s="8"/>
       <c r="BE44" s="8"/>
-      <c r="BF44" s="7"/>
+      <c r="BF44" s="7">
+        <v>48.730511693763432</v>
+      </c>
       <c r="BG44" s="8"/>
       <c r="BH44" s="1">
         <v>80.345136998100003</v>
@@ -6265,7 +6553,9 @@
       <c r="C45" s="2">
         <v>65536</v>
       </c>
-      <c r="D45" s="7"/>
+      <c r="D45" s="7">
+        <v>25.333038254103748</v>
+      </c>
       <c r="E45" s="8"/>
       <c r="F45" s="8">
         <v>33.852641887254997</v>
@@ -6282,7 +6572,9 @@
       <c r="L45" s="9">
         <v>48.31765650862026</v>
       </c>
-      <c r="M45" s="7"/>
+      <c r="M45" s="7">
+        <v>76.201019508680218</v>
+      </c>
       <c r="N45" s="8"/>
       <c r="O45" s="8">
         <v>151.59931210296139</v>
@@ -6299,7 +6591,9 @@
       <c r="U45" s="8">
         <v>281.58226707514871</v>
       </c>
-      <c r="V45" s="7"/>
+      <c r="V45" s="7">
+        <v>48.074815181180512</v>
+      </c>
       <c r="W45" s="8"/>
       <c r="X45" s="8">
         <v>86.73929637082783</v>
@@ -6379,7 +6673,9 @@
       </c>
       <c r="BD45" s="8"/>
       <c r="BE45" s="8"/>
-      <c r="BF45" s="7"/>
+      <c r="BF45" s="7">
+        <v>49.006462580233375</v>
+      </c>
       <c r="BG45" s="8"/>
       <c r="BH45" s="1">
         <v>78.516601550231783</v>
@@ -6407,7 +6703,9 @@
       <c r="C46" s="2">
         <v>131072</v>
       </c>
-      <c r="D46" s="7"/>
+      <c r="D46" s="7">
+        <v>25.334347517933171</v>
+      </c>
       <c r="E46" s="8"/>
       <c r="F46" s="8">
         <v>33.856492889865642</v>
@@ -6424,7 +6722,9 @@
       <c r="L46" s="9">
         <v>48.323895354411313</v>
       </c>
-      <c r="M46" s="7"/>
+      <c r="M46" s="7">
+        <v>76.219326294326109</v>
+      </c>
       <c r="N46" s="8"/>
       <c r="O46" s="8">
         <v>151.60280550087748</v>
@@ -6441,7 +6741,9 @@
       <c r="U46" s="8">
         <v>281.56894722496907</v>
       </c>
-      <c r="V46" s="7"/>
+      <c r="V46" s="7">
+        <v>48.210149972134531</v>
+      </c>
       <c r="W46" s="8"/>
       <c r="X46" s="8">
         <v>86.363721157108046</v>
@@ -6521,7 +6823,9 @@
       </c>
       <c r="BD46" s="8"/>
       <c r="BE46" s="8"/>
-      <c r="BF46" s="7"/>
+      <c r="BF46" s="7">
+        <v>48.986316358333731</v>
+      </c>
       <c r="BG46" s="8"/>
       <c r="BH46" s="1">
         <v>74.3624903700575</v>
@@ -6549,7 +6853,9 @@
       <c r="C47" s="2">
         <v>262144</v>
       </c>
-      <c r="D47" s="7"/>
+      <c r="D47" s="7">
+        <v>25.335328270861819</v>
+      </c>
       <c r="E47" s="8"/>
       <c r="F47" s="8">
         <v>33.857721727448052</v>
@@ -6566,7 +6872,9 @@
       <c r="L47" s="9">
         <v>48.327202222278068</v>
       </c>
-      <c r="M47" s="7"/>
+      <c r="M47" s="7">
+        <v>76.234224470759145</v>
+      </c>
       <c r="N47" s="8"/>
       <c r="O47" s="8">
         <v>151.6103444344449</v>
@@ -6583,7 +6891,9 @@
       <c r="U47" s="8">
         <v>281.57465557788129</v>
       </c>
-      <c r="V47" s="7"/>
+      <c r="V47" s="7">
+        <v>48.258178940941448</v>
+      </c>
       <c r="W47" s="8"/>
       <c r="X47" s="8">
         <v>86.297777038301717</v>
@@ -6663,7 +6973,9 @@
       </c>
       <c r="BD47" s="8"/>
       <c r="BE47" s="8"/>
-      <c r="BF47" s="7"/>
+      <c r="BF47" s="7">
+        <v>48.999479625526376</v>
+      </c>
       <c r="BG47" s="8"/>
       <c r="BH47" s="1">
         <v>57.110574982415656</v>
@@ -6691,7 +7003,9 @@
       <c r="C48" s="2">
         <v>524288</v>
       </c>
-      <c r="D48" s="7"/>
+      <c r="D48" s="7">
+        <v>25.335629957517725</v>
+      </c>
       <c r="E48" s="8"/>
       <c r="F48" s="8">
         <v>33.85864799980714</v>
@@ -6708,7 +7022,9 @@
       <c r="L48" s="9">
         <v>48.32887451137092</v>
       </c>
-      <c r="M48" s="7"/>
+      <c r="M48" s="7">
+        <v>76.243780032424951</v>
+      </c>
       <c r="N48" s="8"/>
       <c r="O48" s="8">
         <v>151.61540145635689</v>
@@ -6725,7 +7041,9 @@
       <c r="U48" s="8">
         <v>276.63205999596119</v>
       </c>
-      <c r="V48" s="7"/>
+      <c r="V48" s="7">
+        <v>48.159980520251082</v>
+      </c>
       <c r="W48" s="8"/>
       <c r="X48" s="8">
         <v>86.239518880072907</v>
@@ -6805,7 +7123,9 @@
       </c>
       <c r="BD48" s="8"/>
       <c r="BE48" s="8"/>
-      <c r="BF48" s="7"/>
+      <c r="BF48" s="7">
+        <v>48.699214754381615</v>
+      </c>
       <c r="BG48" s="8"/>
       <c r="BH48" s="1">
         <v>70.47861037605837</v>
@@ -6833,7 +7153,9 @@
       <c r="C49" s="2">
         <v>1048576</v>
       </c>
-      <c r="D49" s="7"/>
+      <c r="D49" s="7">
+        <v>25.335783371147414</v>
+      </c>
       <c r="E49" s="8"/>
       <c r="F49" s="8">
         <v>33.859042368767767</v>
@@ -6850,7 +7172,9 @@
       <c r="L49" s="9">
         <v>48.32961960481353</v>
       </c>
-      <c r="M49" s="7"/>
+      <c r="M49" s="7">
+        <v>76.246599496970688</v>
+      </c>
       <c r="N49" s="8"/>
       <c r="O49" s="8">
         <v>151.63464420977803</v>
@@ -6867,7 +7191,9 @@
       <c r="U49" s="8">
         <v>271.09182503625175</v>
       </c>
-      <c r="V49" s="7"/>
+      <c r="V49" s="7">
+        <v>48.125529862083781</v>
+      </c>
       <c r="W49" s="8"/>
       <c r="X49" s="8">
         <v>86.04537602904891</v>
@@ -6947,7 +7273,9 @@
       </c>
       <c r="BD49" s="8"/>
       <c r="BE49" s="8"/>
-      <c r="BF49" s="7"/>
+      <c r="BF49" s="7">
+        <v>48.366856804841909</v>
+      </c>
       <c r="BG49" s="8"/>
       <c r="BH49" s="1">
         <v>78.321740540907172</v>
@@ -6975,7 +7303,9 @@
       <c r="C50" s="2">
         <v>2097152</v>
       </c>
-      <c r="D50" s="10"/>
+      <c r="D50" s="10">
+        <v>25.335859757706078</v>
+      </c>
       <c r="E50" s="11"/>
       <c r="F50" s="11">
         <v>33.859238983469126</v>
@@ -6992,7 +7322,9 @@
       <c r="L50" s="12">
         <v>48.33008559185663</v>
       </c>
-      <c r="M50" s="10"/>
+      <c r="M50" s="10">
+        <v>76.247448283833862</v>
+      </c>
       <c r="N50" s="11"/>
       <c r="O50" s="11">
         <v>151.64802735487777</v>
@@ -7009,7 +7341,9 @@
       <c r="U50" s="11">
         <v>270.89167380579102</v>
       </c>
-      <c r="V50" s="10"/>
+      <c r="V50" s="10">
+        <v>48.139303977392053</v>
+      </c>
       <c r="W50" s="11"/>
       <c r="X50" s="11">
         <v>86.097645319803021</v>
@@ -7089,7 +7423,9 @@
       </c>
       <c r="BD50" s="11"/>
       <c r="BE50" s="11"/>
-      <c r="BF50" s="10"/>
+      <c r="BF50" s="10">
+        <v>48.717224330297718</v>
+      </c>
       <c r="BG50" s="11"/>
       <c r="BH50" s="11">
         <v>79.993126990528978</v>

</xml_diff>

<commit_message>
add main results file these are the same results we used in the paper
</commit_message>
<xml_diff>
--- a/results/Zynq7000_HPS-FPGA.xlsx
+++ b/results/Zynq7000_HPS-FPGA.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="45" yWindow="150" windowWidth="18915" windowHeight="7620"/>
+    <workbookView xWindow="-120" yWindow="15" windowWidth="18915" windowHeight="7620"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -324,22 +324,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -360,6 +348,15 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -369,10 +366,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -678,8 +678,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BO54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="BF52" sqref="BF52"/>
+    <sheetView tabSelected="1" topLeftCell="AU25" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="BM25" sqref="BM25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -717,233 +717,233 @@
     </row>
     <row r="4" spans="1:67" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="1:67" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="D5" s="33" t="s">
+      <c r="D5" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="34"/>
-      <c r="F5" s="34"/>
-      <c r="G5" s="34"/>
-      <c r="H5" s="34"/>
-      <c r="I5" s="34"/>
-      <c r="J5" s="34"/>
-      <c r="K5" s="34"/>
-      <c r="L5" s="34"/>
-      <c r="M5" s="34"/>
-      <c r="N5" s="34"/>
-      <c r="O5" s="34"/>
-      <c r="P5" s="34"/>
-      <c r="Q5" s="34"/>
-      <c r="R5" s="34"/>
-      <c r="S5" s="34"/>
-      <c r="T5" s="34"/>
-      <c r="U5" s="34"/>
-      <c r="V5" s="34"/>
-      <c r="W5" s="34"/>
-      <c r="X5" s="34"/>
-      <c r="Y5" s="34"/>
-      <c r="Z5" s="34"/>
-      <c r="AA5" s="34"/>
-      <c r="AB5" s="34"/>
-      <c r="AC5" s="34"/>
-      <c r="AD5" s="34"/>
-      <c r="AE5" s="34"/>
-      <c r="AF5" s="34"/>
-      <c r="AG5" s="34"/>
-      <c r="AH5" s="34"/>
-      <c r="AI5" s="34"/>
-      <c r="AJ5" s="34"/>
-      <c r="AK5" s="34"/>
-      <c r="AL5" s="34"/>
-      <c r="AM5" s="34"/>
-      <c r="AN5" s="21" t="s">
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="19"/>
+      <c r="J5" s="19"/>
+      <c r="K5" s="19"/>
+      <c r="L5" s="19"/>
+      <c r="M5" s="19"/>
+      <c r="N5" s="19"/>
+      <c r="O5" s="19"/>
+      <c r="P5" s="19"/>
+      <c r="Q5" s="19"/>
+      <c r="R5" s="19"/>
+      <c r="S5" s="19"/>
+      <c r="T5" s="19"/>
+      <c r="U5" s="19"/>
+      <c r="V5" s="19"/>
+      <c r="W5" s="19"/>
+      <c r="X5" s="19"/>
+      <c r="Y5" s="19"/>
+      <c r="Z5" s="19"/>
+      <c r="AA5" s="19"/>
+      <c r="AB5" s="19"/>
+      <c r="AC5" s="19"/>
+      <c r="AD5" s="19"/>
+      <c r="AE5" s="19"/>
+      <c r="AF5" s="19"/>
+      <c r="AG5" s="19"/>
+      <c r="AH5" s="19"/>
+      <c r="AI5" s="19"/>
+      <c r="AJ5" s="19"/>
+      <c r="AK5" s="19"/>
+      <c r="AL5" s="19"/>
+      <c r="AM5" s="19"/>
+      <c r="AN5" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="AO5" s="22"/>
-      <c r="AP5" s="22"/>
-      <c r="AQ5" s="22"/>
-      <c r="AR5" s="22"/>
-      <c r="AS5" s="22"/>
-      <c r="AT5" s="22"/>
-      <c r="AU5" s="22"/>
-      <c r="AV5" s="22"/>
-      <c r="AW5" s="22"/>
-      <c r="AX5" s="22"/>
-      <c r="AY5" s="22"/>
-      <c r="AZ5" s="22"/>
-      <c r="BA5" s="22"/>
-      <c r="BB5" s="22"/>
-      <c r="BC5" s="22"/>
-      <c r="BD5" s="22"/>
-      <c r="BE5" s="22"/>
-      <c r="BF5" s="22"/>
-      <c r="BG5" s="22"/>
-      <c r="BH5" s="22"/>
-      <c r="BI5" s="22"/>
-      <c r="BJ5" s="22"/>
-      <c r="BK5" s="22"/>
-      <c r="BL5" s="22"/>
-      <c r="BM5" s="22"/>
-      <c r="BN5" s="23"/>
+      <c r="AO5" s="33"/>
+      <c r="AP5" s="33"/>
+      <c r="AQ5" s="33"/>
+      <c r="AR5" s="33"/>
+      <c r="AS5" s="33"/>
+      <c r="AT5" s="33"/>
+      <c r="AU5" s="33"/>
+      <c r="AV5" s="33"/>
+      <c r="AW5" s="33"/>
+      <c r="AX5" s="33"/>
+      <c r="AY5" s="33"/>
+      <c r="AZ5" s="33"/>
+      <c r="BA5" s="33"/>
+      <c r="BB5" s="33"/>
+      <c r="BC5" s="33"/>
+      <c r="BD5" s="33"/>
+      <c r="BE5" s="33"/>
+      <c r="BF5" s="33"/>
+      <c r="BG5" s="33"/>
+      <c r="BH5" s="33"/>
+      <c r="BI5" s="33"/>
+      <c r="BJ5" s="33"/>
+      <c r="BK5" s="33"/>
+      <c r="BL5" s="33"/>
+      <c r="BM5" s="33"/>
+      <c r="BN5" s="34"/>
     </row>
     <row r="6" spans="1:67" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D6" s="24" t="s">
+      <c r="D6" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="25"/>
-      <c r="H6" s="25"/>
-      <c r="I6" s="25"/>
-      <c r="J6" s="25"/>
-      <c r="K6" s="25"/>
-      <c r="L6" s="26"/>
-      <c r="M6" s="24" t="s">
+      <c r="E6" s="21"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="21"/>
+      <c r="H6" s="21"/>
+      <c r="I6" s="21"/>
+      <c r="J6" s="21"/>
+      <c r="K6" s="21"/>
+      <c r="L6" s="22"/>
+      <c r="M6" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="N6" s="25"/>
-      <c r="O6" s="25"/>
-      <c r="P6" s="25"/>
-      <c r="Q6" s="25"/>
-      <c r="R6" s="25"/>
-      <c r="S6" s="25"/>
-      <c r="T6" s="25"/>
-      <c r="U6" s="25"/>
-      <c r="V6" s="24" t="s">
+      <c r="N6" s="21"/>
+      <c r="O6" s="21"/>
+      <c r="P6" s="21"/>
+      <c r="Q6" s="21"/>
+      <c r="R6" s="21"/>
+      <c r="S6" s="21"/>
+      <c r="T6" s="21"/>
+      <c r="U6" s="21"/>
+      <c r="V6" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="W6" s="25"/>
-      <c r="X6" s="25"/>
-      <c r="Y6" s="25"/>
-      <c r="Z6" s="25"/>
-      <c r="AA6" s="25"/>
-      <c r="AB6" s="25"/>
-      <c r="AC6" s="25"/>
-      <c r="AD6" s="26"/>
-      <c r="AE6" s="24" t="s">
+      <c r="W6" s="21"/>
+      <c r="X6" s="21"/>
+      <c r="Y6" s="21"/>
+      <c r="Z6" s="21"/>
+      <c r="AA6" s="21"/>
+      <c r="AB6" s="21"/>
+      <c r="AC6" s="21"/>
+      <c r="AD6" s="22"/>
+      <c r="AE6" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="AF6" s="25"/>
-      <c r="AG6" s="25"/>
-      <c r="AH6" s="25"/>
-      <c r="AI6" s="25"/>
-      <c r="AJ6" s="25"/>
-      <c r="AK6" s="25"/>
-      <c r="AL6" s="25"/>
-      <c r="AM6" s="26"/>
-      <c r="AN6" s="27" t="s">
+      <c r="AF6" s="21"/>
+      <c r="AG6" s="21"/>
+      <c r="AH6" s="21"/>
+      <c r="AI6" s="21"/>
+      <c r="AJ6" s="21"/>
+      <c r="AK6" s="21"/>
+      <c r="AL6" s="21"/>
+      <c r="AM6" s="22"/>
+      <c r="AN6" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="AO6" s="28"/>
-      <c r="AP6" s="28"/>
-      <c r="AQ6" s="28"/>
-      <c r="AR6" s="28"/>
-      <c r="AS6" s="28"/>
-      <c r="AT6" s="28"/>
-      <c r="AU6" s="28"/>
-      <c r="AV6" s="29"/>
-      <c r="AW6" s="27" t="s">
+      <c r="AO6" s="24"/>
+      <c r="AP6" s="24"/>
+      <c r="AQ6" s="24"/>
+      <c r="AR6" s="24"/>
+      <c r="AS6" s="24"/>
+      <c r="AT6" s="24"/>
+      <c r="AU6" s="24"/>
+      <c r="AV6" s="25"/>
+      <c r="AW6" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="AX6" s="28"/>
-      <c r="AY6" s="28"/>
-      <c r="AZ6" s="28"/>
-      <c r="BA6" s="28"/>
-      <c r="BB6" s="28"/>
-      <c r="BC6" s="28"/>
-      <c r="BD6" s="28"/>
-      <c r="BE6" s="29"/>
-      <c r="BF6" s="24" t="s">
+      <c r="AX6" s="24"/>
+      <c r="AY6" s="24"/>
+      <c r="AZ6" s="24"/>
+      <c r="BA6" s="24"/>
+      <c r="BB6" s="24"/>
+      <c r="BC6" s="24"/>
+      <c r="BD6" s="24"/>
+      <c r="BE6" s="25"/>
+      <c r="BF6" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="BG6" s="25"/>
-      <c r="BH6" s="25"/>
-      <c r="BI6" s="25"/>
-      <c r="BJ6" s="25"/>
-      <c r="BK6" s="25"/>
-      <c r="BL6" s="25"/>
-      <c r="BM6" s="25"/>
-      <c r="BN6" s="26"/>
+      <c r="BG6" s="21"/>
+      <c r="BH6" s="21"/>
+      <c r="BI6" s="21"/>
+      <c r="BJ6" s="21"/>
+      <c r="BK6" s="21"/>
+      <c r="BL6" s="21"/>
+      <c r="BM6" s="21"/>
+      <c r="BN6" s="22"/>
     </row>
     <row r="7" spans="1:67" x14ac:dyDescent="0.25">
       <c r="B7" s="8"/>
       <c r="C7" s="1"/>
-      <c r="D7" s="18" t="s">
+      <c r="D7" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="E7" s="19"/>
-      <c r="F7" s="19"/>
-      <c r="G7" s="19"/>
-      <c r="H7" s="19"/>
-      <c r="I7" s="19"/>
-      <c r="J7" s="19"/>
-      <c r="K7" s="19"/>
-      <c r="L7" s="20"/>
-      <c r="M7" s="18" t="s">
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="27"/>
+      <c r="I7" s="27"/>
+      <c r="J7" s="27"/>
+      <c r="K7" s="27"/>
+      <c r="L7" s="28"/>
+      <c r="M7" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="N7" s="19"/>
-      <c r="O7" s="19"/>
-      <c r="P7" s="19"/>
-      <c r="Q7" s="19"/>
-      <c r="R7" s="19"/>
-      <c r="S7" s="19"/>
-      <c r="T7" s="19"/>
-      <c r="U7" s="20"/>
-      <c r="V7" s="18" t="s">
+      <c r="N7" s="27"/>
+      <c r="O7" s="27"/>
+      <c r="P7" s="27"/>
+      <c r="Q7" s="27"/>
+      <c r="R7" s="27"/>
+      <c r="S7" s="27"/>
+      <c r="T7" s="27"/>
+      <c r="U7" s="28"/>
+      <c r="V7" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="W7" s="19"/>
-      <c r="X7" s="19"/>
-      <c r="Y7" s="19"/>
-      <c r="Z7" s="19"/>
-      <c r="AA7" s="19"/>
-      <c r="AB7" s="19"/>
-      <c r="AC7" s="19"/>
-      <c r="AD7" s="20"/>
-      <c r="AE7" s="18" t="s">
+      <c r="W7" s="27"/>
+      <c r="X7" s="27"/>
+      <c r="Y7" s="27"/>
+      <c r="Z7" s="27"/>
+      <c r="AA7" s="27"/>
+      <c r="AB7" s="27"/>
+      <c r="AC7" s="27"/>
+      <c r="AD7" s="28"/>
+      <c r="AE7" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="AF7" s="19"/>
-      <c r="AG7" s="19"/>
-      <c r="AH7" s="19"/>
-      <c r="AI7" s="19"/>
-      <c r="AJ7" s="19"/>
-      <c r="AK7" s="19"/>
-      <c r="AL7" s="19"/>
-      <c r="AM7" s="20"/>
-      <c r="AN7" s="18" t="s">
+      <c r="AF7" s="27"/>
+      <c r="AG7" s="27"/>
+      <c r="AH7" s="27"/>
+      <c r="AI7" s="27"/>
+      <c r="AJ7" s="27"/>
+      <c r="AK7" s="27"/>
+      <c r="AL7" s="27"/>
+      <c r="AM7" s="28"/>
+      <c r="AN7" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="AO7" s="19"/>
-      <c r="AP7" s="19"/>
-      <c r="AQ7" s="19"/>
-      <c r="AR7" s="19"/>
-      <c r="AS7" s="19"/>
-      <c r="AT7" s="19"/>
-      <c r="AU7" s="19"/>
-      <c r="AV7" s="20"/>
-      <c r="AW7" s="18" t="s">
+      <c r="AO7" s="27"/>
+      <c r="AP7" s="27"/>
+      <c r="AQ7" s="27"/>
+      <c r="AR7" s="27"/>
+      <c r="AS7" s="27"/>
+      <c r="AT7" s="27"/>
+      <c r="AU7" s="27"/>
+      <c r="AV7" s="28"/>
+      <c r="AW7" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="AX7" s="19"/>
-      <c r="AY7" s="19"/>
-      <c r="AZ7" s="19"/>
-      <c r="BA7" s="19"/>
-      <c r="BB7" s="19"/>
-      <c r="BC7" s="19"/>
-      <c r="BD7" s="19"/>
-      <c r="BE7" s="20"/>
-      <c r="BF7" s="18" t="s">
+      <c r="AX7" s="27"/>
+      <c r="AY7" s="27"/>
+      <c r="AZ7" s="27"/>
+      <c r="BA7" s="27"/>
+      <c r="BB7" s="27"/>
+      <c r="BC7" s="27"/>
+      <c r="BD7" s="27"/>
+      <c r="BE7" s="28"/>
+      <c r="BF7" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="BG7" s="19"/>
-      <c r="BH7" s="19"/>
-      <c r="BI7" s="19"/>
-      <c r="BJ7" s="19"/>
-      <c r="BK7" s="19"/>
-      <c r="BL7" s="19"/>
-      <c r="BM7" s="19"/>
-      <c r="BN7" s="20"/>
+      <c r="BG7" s="27"/>
+      <c r="BH7" s="27"/>
+      <c r="BI7" s="27"/>
+      <c r="BJ7" s="27"/>
+      <c r="BK7" s="27"/>
+      <c r="BL7" s="27"/>
+      <c r="BM7" s="27"/>
+      <c r="BN7" s="28"/>
       <c r="BO7" s="17"/>
     </row>
     <row r="8" spans="1:67" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1140,10 +1140,10 @@
       </c>
     </row>
     <row r="9" spans="1:67" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="30" t="s">
+      <c r="A9" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="30" t="s">
+      <c r="B9" s="29" t="s">
         <v>10</v>
       </c>
       <c r="C9" s="2">
@@ -1235,37 +1235,37 @@
       <c r="AM9" s="6">
         <v>11.559688683712121</v>
       </c>
-      <c r="AN9" s="4">
-        <v>8.8722143120871705E-2</v>
+      <c r="AN9" s="1">
+        <v>8.6556027991128145E-2</v>
       </c>
       <c r="AO9" s="5"/>
-      <c r="AP9" s="5">
-        <v>8.9095134193409004E-2</v>
+      <c r="AP9" s="1">
+        <v>8.6250729529370546E-2</v>
       </c>
       <c r="AQ9" s="5"/>
-      <c r="AR9" s="5">
-        <v>8.8356354880831059E-2</v>
+      <c r="AR9" s="1">
+        <v>8.670160610993681E-2</v>
       </c>
       <c r="AS9" s="5"/>
-      <c r="AT9" s="5">
-        <v>8.8672646806717811E-2</v>
+      <c r="AT9" s="1">
+        <v>8.6607121319189032E-2</v>
       </c>
       <c r="AU9" s="5"/>
       <c r="AV9" s="6"/>
-      <c r="AW9" s="4">
-        <v>1.0276662892308728</v>
+      <c r="AW9" s="1">
+        <v>1.0188828166733439</v>
       </c>
       <c r="AX9" s="5"/>
-      <c r="AY9" s="5">
-        <v>1.0282202872304582</v>
+      <c r="AY9" s="1">
+        <v>1.0183388322544047</v>
       </c>
       <c r="AZ9" s="5"/>
-      <c r="BA9" s="5">
-        <v>1.0326738672509475</v>
+      <c r="BA9" s="1">
+        <v>1.0221589672092712</v>
       </c>
       <c r="BB9" s="5"/>
-      <c r="BC9" s="5">
-        <v>1.0172526041666667</v>
+      <c r="BC9" s="1">
+        <v>1.0199725309157754</v>
       </c>
       <c r="BD9" s="5"/>
       <c r="BE9" s="5"/>
@@ -1294,8 +1294,8 @@
       <c r="BN9" s="6"/>
     </row>
     <row r="10" spans="1:67" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="31"/>
-      <c r="B10" s="31"/>
+      <c r="A10" s="30"/>
+      <c r="B10" s="30"/>
       <c r="C10" s="2">
         <v>4</v>
       </c>
@@ -1385,37 +1385,37 @@
       <c r="AM10" s="9">
         <v>20.732050356657609</v>
       </c>
-      <c r="AN10" s="7">
-        <v>0.17678641512767634</v>
+      <c r="AN10" s="1">
+        <v>0.1730335328687744</v>
       </c>
       <c r="AO10" s="8"/>
-      <c r="AP10" s="8">
-        <v>0.17753512661725696</v>
+      <c r="AP10" s="1">
+        <v>0.17239232039158534</v>
       </c>
       <c r="AQ10" s="8"/>
-      <c r="AR10" s="8">
-        <v>0.17742777979651161</v>
+      <c r="AR10" s="1">
+        <v>0.17302568447521205</v>
       </c>
       <c r="AS10" s="8"/>
-      <c r="AT10" s="8">
-        <v>0.1771229635336862</v>
+      <c r="AT10" s="1">
+        <v>0.1729942980193642</v>
       </c>
       <c r="AU10" s="8"/>
       <c r="AV10" s="9"/>
-      <c r="AW10" s="7">
-        <v>2.0675865938346885</v>
+      <c r="AW10" s="1">
+        <v>2.046511408597103</v>
       </c>
       <c r="AX10" s="8"/>
-      <c r="AY10" s="8">
-        <v>2.0653477345018949</v>
+      <c r="AY10" s="1">
+        <v>2.0476099117686526</v>
       </c>
       <c r="AZ10" s="8"/>
-      <c r="BA10" s="8">
-        <v>2.0754609715043526</v>
+      <c r="BA10" s="1">
+        <v>2.0476099117686526</v>
       </c>
       <c r="BB10" s="8"/>
-      <c r="BC10" s="8">
-        <v>2.0653477345018949</v>
+      <c r="BC10" s="1">
+        <v>2.0421291571868307</v>
       </c>
       <c r="BD10" s="8"/>
       <c r="BE10" s="8"/>
@@ -1444,8 +1444,8 @@
       <c r="BN10" s="9"/>
     </row>
     <row r="11" spans="1:67" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="31"/>
-      <c r="B11" s="31"/>
+      <c r="A11" s="30"/>
+      <c r="B11" s="30"/>
       <c r="C11" s="2">
         <v>8</v>
       </c>
@@ -1535,37 +1535,37 @@
       <c r="AM11" s="9">
         <v>27.642733808876812</v>
       </c>
-      <c r="AN11" s="7">
-        <v>0.35321270978009262</v>
+      <c r="AN11" s="1">
+        <v>0.34611416464410472</v>
       </c>
       <c r="AO11" s="8"/>
-      <c r="AP11" s="8">
-        <v>0.35455871973464076</v>
+      <c r="AP11" s="1">
+        <v>0.34542466298048624</v>
       </c>
       <c r="AQ11" s="8"/>
-      <c r="AR11" s="8">
-        <v>0.35535139875407545</v>
+      <c r="AR11" s="1">
+        <v>0.34614557103806542</v>
       </c>
       <c r="AS11" s="8"/>
-      <c r="AT11" s="8">
-        <v>0.35418014629079431</v>
+      <c r="AT11" s="1">
+        <v>0.34583176334934951</v>
       </c>
       <c r="AU11" s="8"/>
       <c r="AV11" s="9"/>
-      <c r="AW11" s="7">
-        <v>4.104031485341582</v>
+      <c r="AW11" s="1">
+        <v>4.03244954082981</v>
       </c>
       <c r="AX11" s="8"/>
-      <c r="AY11" s="8">
-        <v>4.093022817194206</v>
+      <c r="AY11" s="1">
+        <v>4.0388536428004231</v>
       </c>
       <c r="AZ11" s="8"/>
-      <c r="BA11" s="8">
-        <v>4.0798901236631018</v>
+      <c r="BA11" s="1">
+        <v>4.0452781183722166</v>
       </c>
       <c r="BB11" s="8"/>
-      <c r="BC11" s="8">
-        <v>4.077709530331374</v>
+      <c r="BC11" s="1">
+        <v>4.0388536428004231</v>
       </c>
       <c r="BD11" s="8"/>
       <c r="BE11" s="8"/>
@@ -1594,8 +1594,8 @@
       <c r="BN11" s="9"/>
     </row>
     <row r="12" spans="1:67" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="31"/>
-      <c r="B12" s="31"/>
+      <c r="A12" s="30"/>
+      <c r="B12" s="30"/>
       <c r="C12" s="2">
         <v>16</v>
       </c>
@@ -1685,37 +1685,37 @@
       <c r="AM12" s="9">
         <v>28.574511352996254</v>
       </c>
-      <c r="AN12" s="7">
-        <v>0.70948012565676299</v>
+      <c r="AN12" s="1">
+        <v>0.69326620002271688</v>
       </c>
       <c r="AO12" s="8"/>
-      <c r="AP12" s="8">
-        <v>0.70888683217189308</v>
+      <c r="AP12" s="1">
+        <v>0.68789058978000184</v>
       </c>
       <c r="AQ12" s="8"/>
-      <c r="AR12" s="8">
-        <v>0.70915039561741877</v>
+      <c r="AR12" s="1">
+        <v>0.69247964885409574</v>
       </c>
       <c r="AS12" s="8"/>
-      <c r="AT12" s="8">
-        <v>0.70790021166782646</v>
+      <c r="AT12" s="1">
+        <v>0.69141279906203268</v>
       </c>
       <c r="AU12" s="8"/>
       <c r="AV12" s="9"/>
-      <c r="AW12" s="7">
-        <v>8.4024168846365637</v>
+      <c r="AW12" s="1">
+        <v>8.2301990628371087</v>
       </c>
       <c r="AX12" s="8"/>
-      <c r="AY12" s="8">
-        <v>8.4489418950719823</v>
+      <c r="AY12" s="1">
+        <v>8.1948383794307205</v>
       </c>
       <c r="AZ12" s="8"/>
-      <c r="BA12" s="8">
-        <v>8.4442662216380739</v>
+      <c r="BA12" s="1">
+        <v>8.2124806579655534</v>
       </c>
       <c r="BB12" s="8"/>
-      <c r="BC12" s="8">
-        <v>8.4349303828081812</v>
+      <c r="BC12" s="1">
+        <v>8.2036500336021501</v>
       </c>
       <c r="BD12" s="8"/>
       <c r="BE12" s="8"/>
@@ -1744,8 +1744,8 @@
       <c r="BN12" s="9"/>
     </row>
     <row r="13" spans="1:67" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="31"/>
-      <c r="B13" s="31"/>
+      <c r="A13" s="30"/>
+      <c r="B13" s="30"/>
       <c r="C13" s="2">
         <v>32</v>
       </c>
@@ -1835,37 +1835,37 @@
       <c r="AM13" s="9">
         <v>30.12594089338598</v>
       </c>
-      <c r="AN13" s="7">
-        <v>1.4153407905110842</v>
+      <c r="AN13" s="1">
+        <v>1.387099592063997</v>
       </c>
       <c r="AO13" s="8"/>
-      <c r="AP13" s="8">
-        <v>1.4198184667814273</v>
+      <c r="AP13" s="1">
+        <v>1.3814484688334616</v>
       </c>
       <c r="AQ13" s="8"/>
-      <c r="AR13" s="8">
-        <v>1.417444408964236</v>
+      <c r="AR13" s="1">
+        <v>1.38766724831757</v>
       </c>
       <c r="AS13" s="8"/>
-      <c r="AT13" s="8">
-        <v>1.4133743110874399</v>
+      <c r="AT13" s="1">
+        <v>1.3908927635476962</v>
       </c>
       <c r="AU13" s="8"/>
       <c r="AV13" s="9"/>
-      <c r="AW13" s="7">
-        <v>16.612726252041373</v>
+      <c r="AW13" s="1">
+        <v>16.138327934955051</v>
       </c>
       <c r="AX13" s="8"/>
-      <c r="AY13" s="8">
-        <v>16.540692750677508</v>
+      <c r="AY13" s="1">
+        <v>16.078808285036882</v>
       </c>
       <c r="AZ13" s="8"/>
-      <c r="BA13" s="8">
-        <v>16.522781876015159</v>
+      <c r="BA13" s="1">
+        <v>16.155414571201693</v>
       </c>
       <c r="BB13" s="8"/>
-      <c r="BC13" s="8">
-        <v>16.630832765667574</v>
+      <c r="BC13" s="1">
+        <v>16.095769053270043</v>
       </c>
       <c r="BD13" s="8"/>
       <c r="BE13" s="8"/>
@@ -1894,8 +1894,8 @@
       <c r="BN13" s="9"/>
     </row>
     <row r="14" spans="1:67" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="31"/>
-      <c r="B14" s="31"/>
+      <c r="A14" s="30"/>
+      <c r="B14" s="30"/>
       <c r="C14" s="2">
         <v>64</v>
       </c>
@@ -1985,37 +1985,37 @@
       <c r="AM14" s="9">
         <v>30.111078564380861</v>
       </c>
-      <c r="AN14" s="7">
-        <v>2.8296317222994904</v>
+      <c r="AN14" s="1">
+        <v>2.7625217819317465</v>
       </c>
       <c r="AO14" s="8"/>
-      <c r="AP14" s="8">
-        <v>2.8347571524778226</v>
+      <c r="AP14" s="1">
+        <v>2.7406895487202516</v>
       </c>
       <c r="AQ14" s="8"/>
-      <c r="AR14" s="8">
-        <v>2.8405620258761113</v>
+      <c r="AR14" s="1">
+        <v>2.7718054609445959</v>
       </c>
       <c r="AS14" s="8"/>
-      <c r="AT14" s="8">
-        <v>2.8471873979568034</v>
+      <c r="AT14" s="1">
+        <v>2.7702957629811187</v>
       </c>
       <c r="AU14" s="8"/>
       <c r="AV14" s="9"/>
-      <c r="AW14" s="7">
-        <v>32.174568397469692</v>
+      <c r="AW14" s="1">
+        <v>31.380543059125962</v>
       </c>
       <c r="AX14" s="8"/>
-      <c r="AY14" s="8">
-        <v>32.157616570073763</v>
+      <c r="AY14" s="1">
+        <v>31.300080128205128</v>
       </c>
       <c r="AZ14" s="8"/>
-      <c r="BA14" s="8">
-        <v>32.174568397469692</v>
+      <c r="BA14" s="1">
+        <v>31.268010373975407</v>
       </c>
       <c r="BB14" s="8"/>
-      <c r="BC14" s="8">
-        <v>32.225531282998944</v>
+      <c r="BC14" s="1">
+        <v>31.236006269191403</v>
       </c>
       <c r="BD14" s="8"/>
       <c r="BE14" s="8"/>
@@ -2044,8 +2044,8 @@
       <c r="BN14" s="9"/>
     </row>
     <row r="15" spans="1:67" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="31"/>
-      <c r="B15" s="31"/>
+      <c r="A15" s="30"/>
+      <c r="B15" s="30"/>
       <c r="C15" s="2">
         <v>128</v>
       </c>
@@ -2135,37 +2135,37 @@
       <c r="AM15" s="9">
         <v>31.244001151778857</v>
       </c>
-      <c r="AN15" s="7">
-        <v>5.6253600230414751</v>
+      <c r="AN15" s="1">
+        <v>5.5277957025766433</v>
       </c>
       <c r="AO15" s="8"/>
-      <c r="AP15" s="8">
-        <v>5.6188866513233604</v>
+      <c r="AP15" s="1">
+        <v>5.4870460062030837</v>
       </c>
       <c r="AQ15" s="8"/>
-      <c r="AR15" s="8">
-        <v>5.6318483275663205</v>
+      <c r="AR15" s="1">
+        <v>5.5190483994936246</v>
       </c>
       <c r="AS15" s="8"/>
-      <c r="AT15" s="8">
-        <v>5.635228164527744</v>
+      <c r="AT15" s="1">
+        <v>5.5217945673316144</v>
       </c>
       <c r="AU15" s="8"/>
       <c r="AV15" s="9"/>
-      <c r="AW15" s="7">
-        <v>60.25188178677196</v>
+      <c r="AW15" s="1">
+        <v>58.631274015369833</v>
       </c>
       <c r="AX15" s="8"/>
-      <c r="AY15" s="8">
-        <v>60.25188178677196</v>
+      <c r="AY15" s="1">
+        <v>58.772418151179579</v>
       </c>
       <c r="AZ15" s="8"/>
-      <c r="BA15" s="8">
-        <v>60.430847772277225</v>
+      <c r="BA15" s="1">
+        <v>58.57500599808062</v>
       </c>
       <c r="BB15" s="8"/>
-      <c r="BC15" s="8">
-        <v>60.133158866995075</v>
+      <c r="BC15" s="1">
+        <v>58.885823685479984</v>
       </c>
       <c r="BD15" s="8"/>
       <c r="BE15" s="8"/>
@@ -2194,8 +2194,8 @@
       <c r="BN15" s="9"/>
     </row>
     <row r="16" spans="1:67" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="31"/>
-      <c r="B16" s="31"/>
+      <c r="A16" s="30"/>
+      <c r="B16" s="30"/>
       <c r="C16" s="2">
         <v>256</v>
       </c>
@@ -2285,37 +2285,37 @@
       <c r="AM16" s="9">
         <v>31.465475576749583</v>
       </c>
-      <c r="AN16" s="7">
-        <v>11.10689345343706</v>
+      <c r="AN16" s="1">
+        <v>10.858415984700232</v>
       </c>
       <c r="AO16" s="8"/>
-      <c r="AP16" s="8">
-        <v>11.080680116189352</v>
+      <c r="AP16" s="1">
+        <v>10.815603818721481</v>
       </c>
       <c r="AQ16" s="8"/>
-      <c r="AR16" s="8">
-        <v>11.087725373541032</v>
+      <c r="AR16" s="1">
+        <v>10.896702744923008</v>
       </c>
       <c r="AS16" s="8"/>
-      <c r="AT16" s="8">
-        <v>11.100328498681458</v>
+      <c r="AT16" s="1">
+        <v>10.896216415245917</v>
       </c>
       <c r="AU16" s="8"/>
       <c r="AV16" s="9"/>
-      <c r="AW16" s="7">
-        <v>107.07922149122805</v>
+      <c r="AW16" s="1">
+        <v>104.69152015437393</v>
       </c>
       <c r="AX16" s="8"/>
-      <c r="AY16" s="8">
-        <v>106.84491247264769</v>
+      <c r="AY16" s="1">
+        <v>104.51225385273972</v>
       </c>
       <c r="AZ16" s="8"/>
-      <c r="BA16" s="8">
-        <v>106.98537467134094</v>
+      <c r="BA16" s="1">
+        <v>104.46753316217374</v>
       </c>
       <c r="BB16" s="8"/>
-      <c r="BC16" s="8">
-        <v>106.93851292159439</v>
+      <c r="BC16" s="1">
+        <v>104.78138412017167</v>
       </c>
       <c r="BD16" s="8"/>
       <c r="BE16" s="8"/>
@@ -2344,8 +2344,8 @@
       <c r="BN16" s="9"/>
     </row>
     <row r="17" spans="1:66" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="31"/>
-      <c r="B17" s="31"/>
+      <c r="A17" s="30"/>
+      <c r="B17" s="30"/>
       <c r="C17" s="2">
         <v>512</v>
       </c>
@@ -2435,37 +2435,37 @@
       <c r="AM17" s="9">
         <v>31.575352431453698</v>
       </c>
-      <c r="AN17" s="7">
-        <v>20.279987124641774</v>
+      <c r="AN17" s="1">
+        <v>20.218685300207039</v>
       </c>
       <c r="AO17" s="8"/>
-      <c r="AP17" s="8">
-        <v>21.365242408331149</v>
+      <c r="AP17" s="1">
+        <v>21.041163923123328</v>
       </c>
       <c r="AQ17" s="8"/>
-      <c r="AR17" s="8">
-        <v>21.712969139096408</v>
+      <c r="AR17" s="1">
+        <v>21.24254981292961</v>
       </c>
       <c r="AS17" s="8"/>
-      <c r="AT17" s="8">
-        <v>21.716831969400463</v>
+      <c r="AT17" s="1">
+        <v>21.239777719779024</v>
       </c>
       <c r="AU17" s="8"/>
       <c r="AV17" s="9"/>
-      <c r="AW17" s="7">
-        <v>113.05423709191943</v>
+      <c r="AW17" s="1">
+        <v>119.32581867057674</v>
       </c>
       <c r="AX17" s="8"/>
-      <c r="AY17" s="8">
-        <v>155.05914576055892</v>
+      <c r="AY17" s="1">
+        <v>157.05411707944677</v>
       </c>
       <c r="AZ17" s="8"/>
-      <c r="BA17" s="8">
-        <v>173.70375311277127</v>
+      <c r="BA17" s="1">
+        <v>172.05118040873853</v>
       </c>
       <c r="BB17" s="8"/>
-      <c r="BC17" s="8">
-        <v>175.07395123700252</v>
+      <c r="BC17" s="1">
+        <v>172.23324514991182</v>
       </c>
       <c r="BD17" s="8"/>
       <c r="BE17" s="8"/>
@@ -2494,8 +2494,8 @@
       <c r="BN17" s="9"/>
     </row>
     <row r="18" spans="1:66" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="31"/>
-      <c r="B18" s="31"/>
+      <c r="A18" s="30"/>
+      <c r="B18" s="30"/>
       <c r="C18" s="2">
         <v>1024</v>
       </c>
@@ -2585,37 +2585,37 @@
       <c r="AM18" s="9">
         <v>31.688055681744434</v>
       </c>
-      <c r="AN18" s="7">
-        <v>34.300252888904502</v>
+      <c r="AN18" s="1">
+        <v>34.754350688636606</v>
       </c>
       <c r="AO18" s="8"/>
-      <c r="AP18" s="8">
-        <v>38.973640100570698</v>
+      <c r="AP18" s="1">
+        <v>38.792504170970048</v>
       </c>
       <c r="AQ18" s="8"/>
-      <c r="AR18" s="8">
-        <v>40.597069216379133</v>
+      <c r="AR18" s="1">
+        <v>40.254018961253088</v>
       </c>
       <c r="AS18" s="8"/>
-      <c r="AT18" s="8">
-        <v>41.628479474828424</v>
+      <c r="AT18" s="1">
+        <v>40.735932090268221</v>
       </c>
       <c r="AU18" s="8"/>
       <c r="AV18" s="9"/>
-      <c r="AW18" s="7">
-        <v>111.02347658026376</v>
+      <c r="AW18" s="1">
+        <v>122.94630492257333</v>
       </c>
       <c r="AX18" s="8"/>
-      <c r="AY18" s="8">
-        <v>181.01251158480073</v>
+      <c r="AY18" s="1">
+        <v>194.26347722299582</v>
       </c>
       <c r="AZ18" s="8"/>
-      <c r="BA18" s="8">
-        <v>222.90858251540743</v>
+      <c r="BA18" s="1">
+        <v>234.92001443348568</v>
       </c>
       <c r="BB18" s="8"/>
-      <c r="BC18" s="8">
-        <v>258.07677061310784</v>
+      <c r="BC18" s="1">
+        <v>253.98244473342004</v>
       </c>
       <c r="BD18" s="8"/>
       <c r="BE18" s="8"/>
@@ -2644,8 +2644,8 @@
       <c r="BN18" s="9"/>
     </row>
     <row r="19" spans="1:66" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="31"/>
-      <c r="B19" s="31"/>
+      <c r="A19" s="30"/>
+      <c r="B19" s="30"/>
       <c r="C19" s="2">
         <v>2048</v>
       </c>
@@ -2735,37 +2735,37 @@
       <c r="AM19" s="9">
         <v>31.725630654776406</v>
       </c>
-      <c r="AN19" s="7">
-        <v>52.100005335040549</v>
+      <c r="AN19" s="1">
+        <v>54.692531712917592</v>
       </c>
       <c r="AO19" s="8"/>
-      <c r="AP19" s="8">
-        <v>66.218850652652989</v>
+      <c r="AP19" s="1">
+        <v>67.027866433302449</v>
       </c>
       <c r="AQ19" s="8"/>
-      <c r="AR19" s="8">
-        <v>71.816627445212532</v>
+      <c r="AR19" s="1">
+        <v>72.517914825678531</v>
       </c>
       <c r="AS19" s="8"/>
-      <c r="AT19" s="8">
-        <v>76.365538004379104</v>
+      <c r="AT19" s="1">
+        <v>75.186703622435232</v>
       </c>
       <c r="AU19" s="8"/>
       <c r="AV19" s="9"/>
-      <c r="AW19" s="7">
-        <v>110.04141078370613</v>
+      <c r="AW19" s="1">
+        <v>125.07204149590163</v>
       </c>
       <c r="AX19" s="8"/>
-      <c r="AY19" s="8">
-        <v>197.6647100495901</v>
+      <c r="AY19" s="1">
+        <v>220.36838542254316</v>
       </c>
       <c r="AZ19" s="8"/>
-      <c r="BA19" s="8">
-        <v>260.48612963456924</v>
+      <c r="BA19" s="1">
+        <v>285.37770309760373</v>
       </c>
       <c r="BB19" s="8"/>
-      <c r="BC19" s="8">
-        <v>329.30787388298774</v>
+      <c r="BC19" s="1">
+        <v>333.69639501110544</v>
       </c>
       <c r="BD19" s="8"/>
       <c r="BE19" s="8"/>
@@ -2794,8 +2794,8 @@
       <c r="BN19" s="9"/>
     </row>
     <row r="20" spans="1:66" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="31"/>
-      <c r="B20" s="31"/>
+      <c r="A20" s="30"/>
+      <c r="B20" s="30"/>
       <c r="C20" s="2">
         <v>4096</v>
       </c>
@@ -2885,37 +2885,37 @@
       <c r="AM20" s="9">
         <v>31.739808728295053</v>
       </c>
-      <c r="AN20" s="7">
-        <v>70.586375135525842</v>
+      <c r="AN20" s="1">
+        <v>76.500137088245665</v>
       </c>
       <c r="AO20" s="8"/>
-      <c r="AP20" s="8">
-        <v>101.59826258843113</v>
+      <c r="AP20" s="1">
+        <v>106.43732970027249</v>
       </c>
       <c r="AQ20" s="8"/>
-      <c r="AR20" s="8">
-        <v>116.8731113305209</v>
+      <c r="AR20" s="1">
+        <v>120.8392625131473</v>
       </c>
       <c r="AS20" s="8"/>
-      <c r="AT20" s="8">
-        <v>129.62932236012477</v>
+      <c r="AT20" s="1">
+        <v>130.25609390109707</v>
       </c>
       <c r="AU20" s="8"/>
       <c r="AV20" s="9"/>
-      <c r="AW20" s="7">
-        <v>109.50772336071319</v>
+      <c r="AW20" s="1">
+        <v>126.15049249152268</v>
       </c>
       <c r="AX20" s="8"/>
-      <c r="AY20" s="8">
-        <v>207.48127688957348</v>
+      <c r="AY20" s="1">
+        <v>236.14133720227304</v>
       </c>
       <c r="AZ20" s="8"/>
-      <c r="BA20" s="8">
-        <v>283.61649604298265</v>
+      <c r="BA20" s="1">
+        <v>319.73888843414915</v>
       </c>
       <c r="BB20" s="8"/>
-      <c r="BC20" s="8">
-        <v>375.6370804885085</v>
+      <c r="BC20" s="1">
+        <v>394.8898099474323</v>
       </c>
       <c r="BD20" s="8"/>
       <c r="BE20" s="8"/>
@@ -2944,8 +2944,8 @@
       <c r="BN20" s="9"/>
     </row>
     <row r="21" spans="1:66" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="31"/>
-      <c r="B21" s="31"/>
+      <c r="A21" s="30"/>
+      <c r="B21" s="30"/>
       <c r="C21" s="2">
         <v>8192</v>
       </c>
@@ -3035,37 +3035,37 @@
       <c r="AM21" s="9">
         <v>31.701685616666264</v>
       </c>
-      <c r="AN21" s="7">
-        <v>85.480606160074402</v>
+      <c r="AN21" s="1">
+        <v>95.610191893479524</v>
       </c>
       <c r="AO21" s="8"/>
-      <c r="AP21" s="8">
-        <v>138.46058414858925</v>
+      <c r="AP21" s="1">
+        <v>149.33004568304759</v>
       </c>
       <c r="AQ21" s="8"/>
-      <c r="AR21" s="8">
-        <v>169.48692916802256</v>
+      <c r="AR21" s="1">
+        <v>181.62691216813133</v>
       </c>
       <c r="AS21" s="8"/>
-      <c r="AT21" s="8">
-        <v>199.57339191743728</v>
+      <c r="AT21" s="1">
+        <v>205.30036264256057</v>
       </c>
       <c r="AU21" s="8"/>
       <c r="AV21" s="9"/>
-      <c r="AW21" s="7">
-        <v>109.21532719164583</v>
+      <c r="AW21" s="1">
+        <v>126.64742976640136</v>
       </c>
       <c r="AX21" s="8"/>
-      <c r="AY21" s="8">
-        <v>212.48674082737236</v>
+      <c r="AY21" s="1">
+        <v>244.89060247006458</v>
       </c>
       <c r="AZ21" s="8"/>
-      <c r="BA21" s="8">
-        <v>296.55709079866381</v>
+      <c r="BA21" s="1">
+        <v>339.98433352191131</v>
       </c>
       <c r="BB21" s="8"/>
-      <c r="BC21" s="8">
-        <v>403.01779726592724</v>
+      <c r="BC21" s="1">
+        <v>434.38976925215457</v>
       </c>
       <c r="BD21" s="8"/>
       <c r="BE21" s="8"/>
@@ -3094,8 +3094,8 @@
       <c r="BN21" s="9"/>
     </row>
     <row r="22" spans="1:66" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="31"/>
-      <c r="B22" s="31"/>
+      <c r="A22" s="30"/>
+      <c r="B22" s="30"/>
       <c r="C22" s="2">
         <v>16384</v>
       </c>
@@ -3185,37 +3185,37 @@
       <c r="AM22" s="9">
         <v>31.668531309790183</v>
       </c>
-      <c r="AN22" s="7">
-        <v>95.968405665360464</v>
+      <c r="AN22" s="1">
+        <v>109.12455913678109</v>
       </c>
       <c r="AO22" s="8"/>
-      <c r="AP22" s="8">
-        <v>169.36384231006863</v>
+      <c r="AP22" s="1">
+        <v>188.66671496534568</v>
       </c>
       <c r="AQ22" s="8"/>
-      <c r="AR22" s="8">
-        <v>219.72072616821117</v>
+      <c r="AR22" s="1">
+        <v>242.03792056509079</v>
       </c>
       <c r="AS22" s="8"/>
-      <c r="AT22" s="8">
-        <v>274.11799792986091</v>
+      <c r="AT22" s="1">
+        <v>288.10340376885347</v>
       </c>
       <c r="AU22" s="8"/>
       <c r="AV22" s="9"/>
-      <c r="AW22" s="7">
-        <v>109.08875111706881</v>
+      <c r="AW22" s="1">
+        <v>126.93345031520114</v>
       </c>
       <c r="AX22" s="8"/>
-      <c r="AY22" s="8">
-        <v>215.01011407576613</v>
+      <c r="AY22" s="1">
+        <v>249.55280137992716</v>
       </c>
       <c r="AZ22" s="8"/>
-      <c r="BA22" s="8">
-        <v>303.51003282764515</v>
+      <c r="BA22" s="1">
+        <v>351.2814748201439</v>
       </c>
       <c r="BB22" s="8"/>
-      <c r="BC22" s="8">
-        <v>418.01546322801568</v>
+      <c r="BC22" s="1">
+        <v>457.68768856732771</v>
       </c>
       <c r="BD22" s="8"/>
       <c r="BE22" s="8"/>
@@ -3244,8 +3244,8 @@
       <c r="BN22" s="9"/>
     </row>
     <row r="23" spans="1:66" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="31"/>
-      <c r="B23" s="31"/>
+      <c r="A23" s="30"/>
+      <c r="B23" s="30"/>
       <c r="C23" s="2">
         <v>32768</v>
       </c>
@@ -3335,37 +3335,37 @@
       <c r="AM23" s="9">
         <v>31.250593761281461</v>
       </c>
-      <c r="AN23" s="7">
-        <v>102.06881234363057</v>
+      <c r="AN23" s="1">
+        <v>117.48561976014135</v>
       </c>
       <c r="AO23" s="8"/>
-      <c r="AP23" s="8">
-        <v>190.63363570369739</v>
+      <c r="AP23" s="1">
+        <v>216.67533368001386</v>
       </c>
       <c r="AQ23" s="8"/>
-      <c r="AR23" s="8">
-        <v>257.67033039520442</v>
+      <c r="AR23" s="1">
+        <v>290.57063423433476</v>
       </c>
       <c r="AS23" s="8"/>
-      <c r="AT23" s="8">
-        <v>336.88000603688971</v>
+      <c r="AT23" s="1">
+        <v>361.12972935493565</v>
       </c>
       <c r="AU23" s="8"/>
       <c r="AV23" s="9"/>
-      <c r="AW23" s="7">
-        <v>109.03508312834738</v>
+      <c r="AW23" s="1">
+        <v>127.04646444935013</v>
       </c>
       <c r="AX23" s="8"/>
-      <c r="AY23" s="8">
-        <v>216.40524912572278</v>
+      <c r="AY23" s="1">
+        <v>251.83943523495614</v>
       </c>
       <c r="AZ23" s="8"/>
-      <c r="BA23" s="8">
-        <v>307.20078643401325</v>
+      <c r="BA23" s="1">
+        <v>357.07756295991595</v>
       </c>
       <c r="BB23" s="8"/>
-      <c r="BC23" s="8">
-        <v>426.30107086829003</v>
+      <c r="BC23" s="1">
+        <v>469.83296498428876</v>
       </c>
       <c r="BD23" s="8"/>
       <c r="BE23" s="8"/>
@@ -3394,8 +3394,8 @@
       <c r="BN23" s="9"/>
     </row>
     <row r="24" spans="1:66" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="31"/>
-      <c r="B24" s="31"/>
+      <c r="A24" s="30"/>
+      <c r="B24" s="30"/>
       <c r="C24" s="2">
         <v>65536</v>
       </c>
@@ -3485,37 +3485,37 @@
       <c r="AM24" s="9">
         <v>30.813252952649147</v>
       </c>
-      <c r="AN24" s="7">
-        <v>105.43433886765207</v>
+      <c r="AN24" s="1">
+        <v>117.4816446678371</v>
       </c>
       <c r="AO24" s="8"/>
-      <c r="AP24" s="8">
-        <v>203.46310481442535</v>
+      <c r="AP24" s="1">
+        <v>216.62351526242639</v>
       </c>
       <c r="AQ24" s="8"/>
-      <c r="AR24" s="8">
-        <v>282.04862066942547</v>
+      <c r="AR24" s="1">
+        <v>290.54361873239304</v>
       </c>
       <c r="AS24" s="8"/>
-      <c r="AT24" s="8">
-        <v>380.0870855530419</v>
+      <c r="AT24" s="1">
+        <v>360.83575333845243</v>
       </c>
       <c r="AU24" s="8"/>
       <c r="AV24" s="9"/>
-      <c r="AW24" s="7">
-        <v>109.0328005554567</v>
+      <c r="AW24" s="1">
+        <v>127.06196151140712</v>
       </c>
       <c r="AX24" s="8"/>
-      <c r="AY24" s="8">
-        <v>217.235650281885</v>
+      <c r="AY24" s="1">
+        <v>251.92165841035418</v>
       </c>
       <c r="AZ24" s="8"/>
-      <c r="BA24" s="8">
-        <v>309.32325022023815</v>
+      <c r="BA24" s="1">
+        <v>357.19796768644306</v>
       </c>
       <c r="BB24" s="8"/>
-      <c r="BC24" s="8">
-        <v>431.14747313088947</v>
+      <c r="BC24" s="1">
+        <v>470.07679174469939</v>
       </c>
       <c r="BD24" s="8"/>
       <c r="BE24" s="8"/>
@@ -3544,8 +3544,8 @@
       <c r="BN24" s="9"/>
     </row>
     <row r="25" spans="1:66" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="31"/>
-      <c r="B25" s="31"/>
+      <c r="A25" s="30"/>
+      <c r="B25" s="30"/>
       <c r="C25" s="2">
         <v>131072</v>
       </c>
@@ -3635,37 +3635,37 @@
       <c r="AM25" s="9">
         <v>30.544558157083085</v>
       </c>
-      <c r="AN25" s="7">
-        <v>107.21974902001149</v>
+      <c r="AN25" s="1">
+        <v>117.48109259295809</v>
       </c>
       <c r="AO25" s="8"/>
-      <c r="AP25" s="8">
-        <v>210.52844323479479</v>
+      <c r="AP25" s="1">
+        <v>216.67646044267866</v>
       </c>
       <c r="AQ25" s="8"/>
-      <c r="AR25" s="8">
-        <v>296.09486405692599</v>
+      <c r="AR25" s="1">
+        <v>290.46260235902105</v>
       </c>
       <c r="AS25" s="8"/>
-      <c r="AT25" s="8">
-        <v>406.2319226794408</v>
+      <c r="AT25" s="1">
+        <v>360.82533744385557</v>
       </c>
       <c r="AU25" s="8"/>
       <c r="AV25" s="9"/>
-      <c r="AW25" s="7">
-        <v>109.0390778608801</v>
+      <c r="AW25" s="1">
+        <v>127.06622386628975</v>
       </c>
       <c r="AX25" s="8"/>
-      <c r="AY25" s="8">
-        <v>217.66499441906956</v>
+      <c r="AY25" s="1">
+        <v>251.93435195430519</v>
       </c>
       <c r="AZ25" s="8"/>
-      <c r="BA25" s="8">
-        <v>310.43868711753953</v>
+      <c r="BA25" s="1">
+        <v>357.23471749878541</v>
       </c>
       <c r="BB25" s="8"/>
-      <c r="BC25" s="8">
-        <v>433.66789365769381</v>
+      <c r="BC25" s="1">
+        <v>470.1227584546877</v>
       </c>
       <c r="BD25" s="8"/>
       <c r="BE25" s="8"/>
@@ -3694,8 +3694,8 @@
       <c r="BN25" s="9"/>
     </row>
     <row r="26" spans="1:66" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="31"/>
-      <c r="B26" s="31"/>
+      <c r="A26" s="30"/>
+      <c r="B26" s="30"/>
       <c r="C26" s="2">
         <v>262144</v>
       </c>
@@ -3785,37 +3785,37 @@
       <c r="AM26" s="9">
         <v>30.576738440464034</v>
       </c>
-      <c r="AN26" s="7">
-        <v>107.22283005653217</v>
+      <c r="AN26" s="1">
+        <v>117.47220490159822</v>
       </c>
       <c r="AO26" s="8"/>
-      <c r="AP26" s="8">
-        <v>210.56124679209941</v>
+      <c r="AP26" s="1">
+        <v>216.69092160382485</v>
       </c>
       <c r="AQ26" s="8"/>
-      <c r="AR26" s="8">
-        <v>296.1618607494317</v>
+      <c r="AR26" s="1">
+        <v>290.44876658026783</v>
       </c>
       <c r="AS26" s="8"/>
-      <c r="AT26" s="8">
-        <v>406.35870095250482</v>
+      <c r="AT26" s="1">
+        <v>360.79773823113857</v>
       </c>
       <c r="AU26" s="8"/>
       <c r="AV26" s="9"/>
-      <c r="AW26" s="7">
-        <v>109.0489708394328</v>
+      <c r="AW26" s="1">
+        <v>127.06796763934656</v>
       </c>
       <c r="AX26" s="8"/>
-      <c r="AY26" s="8">
-        <v>217.70385135529358</v>
+      <c r="AY26" s="1">
+        <v>251.94628505202692</v>
       </c>
       <c r="AZ26" s="8"/>
-      <c r="BA26" s="8">
-        <v>310.51773242562791</v>
+      <c r="BA26" s="1">
+        <v>357.25615838165822</v>
       </c>
       <c r="BB26" s="8"/>
-      <c r="BC26" s="8">
-        <v>433.80485028527005</v>
+      <c r="BC26" s="1">
+        <v>470.17138687394333</v>
       </c>
       <c r="BD26" s="8"/>
       <c r="BE26" s="8"/>
@@ -3844,8 +3844,8 @@
       <c r="BN26" s="9"/>
     </row>
     <row r="27" spans="1:66" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="31"/>
-      <c r="B27" s="31"/>
+      <c r="A27" s="30"/>
+      <c r="B27" s="30"/>
       <c r="C27" s="2">
         <v>524288</v>
       </c>
@@ -3935,37 +3935,37 @@
       <c r="AM27" s="9">
         <v>30.558958804934466</v>
       </c>
-      <c r="AN27" s="7">
-        <v>107.23007348905857</v>
+      <c r="AN27" s="1">
+        <v>117.45437837035338</v>
       </c>
       <c r="AO27" s="8"/>
-      <c r="AP27" s="8">
-        <v>210.57321820312819</v>
+      <c r="AP27" s="1">
+        <v>216.55971504206457</v>
       </c>
       <c r="AQ27" s="8"/>
-      <c r="AR27" s="8">
-        <v>296.19537046635958</v>
+      <c r="AR27" s="1">
+        <v>290.34959252338189</v>
       </c>
       <c r="AS27" s="8"/>
-      <c r="AT27" s="8">
-        <v>406.3894169693591</v>
+      <c r="AT27" s="1">
+        <v>360.64211607482895</v>
       </c>
       <c r="AU27" s="8"/>
       <c r="AV27" s="9"/>
-      <c r="AW27" s="7">
-        <v>109.05434614285684</v>
+      <c r="AW27" s="1">
+        <v>127.06037934638616</v>
       </c>
       <c r="AX27" s="8"/>
-      <c r="AY27" s="8">
-        <v>217.72537079719274</v>
+      <c r="AY27" s="1">
+        <v>251.91226601129171</v>
       </c>
       <c r="AZ27" s="8"/>
-      <c r="BA27" s="8">
-        <v>310.55997068313877</v>
+      <c r="BA27" s="1">
+        <v>357.19235379759766</v>
       </c>
       <c r="BB27" s="8"/>
-      <c r="BC27" s="8">
-        <v>433.89331604702363</v>
+      <c r="BC27" s="1">
+        <v>470.06795302328908</v>
       </c>
       <c r="BD27" s="8"/>
       <c r="BE27" s="8"/>
@@ -3994,8 +3994,8 @@
       <c r="BN27" s="9"/>
     </row>
     <row r="28" spans="1:66" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="31"/>
-      <c r="B28" s="31"/>
+      <c r="A28" s="30"/>
+      <c r="B28" s="30"/>
       <c r="C28" s="2">
         <v>1048576</v>
       </c>
@@ -4085,37 +4085,37 @@
       <c r="AM28" s="9">
         <v>30.536394985581932</v>
       </c>
-      <c r="AN28" s="7">
-        <v>107.21303573281826</v>
+      <c r="AN28" s="1">
+        <v>117.46665767655179</v>
       </c>
       <c r="AO28" s="8"/>
-      <c r="AP28" s="8">
-        <v>210.52853187928292</v>
+      <c r="AP28" s="1">
+        <v>216.61004841017973</v>
       </c>
       <c r="AQ28" s="8"/>
-      <c r="AR28" s="8">
-        <v>296.11213648163704</v>
+      <c r="AR28" s="1">
+        <v>290.42101463228198</v>
       </c>
       <c r="AS28" s="8"/>
-      <c r="AT28" s="8">
-        <v>406.22796213305429</v>
+      <c r="AT28" s="1">
+        <v>360.7131443148362</v>
       </c>
       <c r="AU28" s="8"/>
       <c r="AV28" s="9"/>
-      <c r="AW28" s="7">
-        <v>109.05652257791733</v>
+      <c r="AW28" s="1">
+        <v>127.058845652599</v>
       </c>
       <c r="AX28" s="8"/>
-      <c r="AY28" s="8">
-        <v>217.73148612843588</v>
+      <c r="AY28" s="1">
+        <v>251.89995541370791</v>
       </c>
       <c r="AZ28" s="8"/>
-      <c r="BA28" s="8">
-        <v>310.57289518537476</v>
+      <c r="BA28" s="1">
+        <v>357.17334443904321</v>
       </c>
       <c r="BB28" s="8"/>
-      <c r="BC28" s="8">
-        <v>433.91967452553047</v>
+      <c r="BC28" s="1">
+        <v>470.03768292103973</v>
       </c>
       <c r="BD28" s="8"/>
       <c r="BE28" s="8"/>
@@ -4144,8 +4144,8 @@
       <c r="BN28" s="9"/>
     </row>
     <row r="29" spans="1:66" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="32"/>
-      <c r="B29" s="32"/>
+      <c r="A29" s="31"/>
+      <c r="B29" s="31"/>
       <c r="C29" s="2">
         <v>2097152</v>
       </c>
@@ -4235,40 +4235,40 @@
       <c r="AM29" s="9">
         <v>30.523305436507457</v>
       </c>
-      <c r="AN29" s="10">
-        <v>107.22281281143201</v>
-      </c>
-      <c r="AO29" s="11"/>
-      <c r="AP29" s="11">
-        <v>210.55840932386326</v>
-      </c>
-      <c r="AQ29" s="11"/>
-      <c r="AR29" s="11">
-        <v>296.16015037827793</v>
-      </c>
-      <c r="AS29" s="11"/>
-      <c r="AT29" s="11">
-        <v>406.31701056322646</v>
-      </c>
-      <c r="AU29" s="11"/>
-      <c r="AV29" s="12"/>
-      <c r="AW29" s="10">
-        <v>109.05678423169769</v>
-      </c>
-      <c r="AX29" s="11"/>
-      <c r="AY29" s="11">
-        <v>217.73369057625726</v>
-      </c>
-      <c r="AZ29" s="11"/>
-      <c r="BA29" s="11">
-        <v>310.58051535867236</v>
-      </c>
-      <c r="BB29" s="11"/>
-      <c r="BC29" s="11">
-        <v>433.93163103400923</v>
-      </c>
-      <c r="BD29" s="11"/>
-      <c r="BE29" s="11"/>
+      <c r="AN29" s="1">
+        <v>117.47042476483301</v>
+      </c>
+      <c r="AO29" s="8"/>
+      <c r="AP29" s="1">
+        <v>216.63890800125478</v>
+      </c>
+      <c r="AQ29" s="8"/>
+      <c r="AR29" s="1">
+        <v>290.44340978820429</v>
+      </c>
+      <c r="AS29" s="8"/>
+      <c r="AT29" s="1">
+        <v>360.72875866741026</v>
+      </c>
+      <c r="AU29" s="8"/>
+      <c r="AV29" s="9"/>
+      <c r="AW29" s="1">
+        <v>127.05788509482043</v>
+      </c>
+      <c r="AX29" s="8"/>
+      <c r="AY29" s="1">
+        <v>251.89894016039918</v>
+      </c>
+      <c r="AZ29" s="8"/>
+      <c r="BA29" s="1">
+        <v>357.16454213291519</v>
+      </c>
+      <c r="BB29" s="8"/>
+      <c r="BC29" s="1">
+        <v>470.0482880606325</v>
+      </c>
+      <c r="BD29" s="8"/>
+      <c r="BE29" s="8"/>
       <c r="BF29" s="7">
         <v>129.34223716671173</v>
       </c>
@@ -4294,10 +4294,10 @@
       <c r="BN29" s="9"/>
     </row>
     <row r="30" spans="1:66" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="30" t="s">
+      <c r="A30" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="B30" s="30" t="s">
+      <c r="B30" s="29" t="s">
         <v>10</v>
       </c>
       <c r="C30" s="15">
@@ -4390,39 +4390,39 @@
         <v>11.559688683712121</v>
       </c>
       <c r="AN30" s="4">
-        <v>8.8176627655332601E-2</v>
+        <v>8.6607121319189032E-2</v>
       </c>
       <c r="AO30" s="5"/>
       <c r="AP30" s="5">
-        <v>8.8693263557893504E-2</v>
+        <v>8.6048390905553551E-2</v>
       </c>
       <c r="AQ30" s="5"/>
       <c r="AR30" s="5">
-        <v>8.9249386215549106E-2</v>
+        <v>8.6583532289822518E-2</v>
       </c>
       <c r="AS30" s="5"/>
       <c r="AT30" s="5">
-        <v>8.8738654173839207E-2</v>
+        <v>8.6563884578946176E-2</v>
       </c>
       <c r="AU30" s="5"/>
       <c r="AV30" s="6"/>
       <c r="AW30" s="4">
-        <v>1.0276662892308728</v>
+        <v>1.0167103586420576</v>
       </c>
       <c r="AX30" s="5"/>
       <c r="AY30" s="5">
-        <v>1.0309992609797296</v>
+        <v>1.0205182626070091</v>
       </c>
       <c r="AZ30" s="5"/>
       <c r="BA30" s="5">
-        <v>1.0293300770709659</v>
+        <v>1.0188828166733439</v>
       </c>
       <c r="BB30" s="5"/>
       <c r="BC30" s="5">
-        <v>1.034353922349512</v>
+        <v>1.0167103586420576</v>
       </c>
       <c r="BD30" s="5"/>
-      <c r="BE30" s="5"/>
+      <c r="BE30" s="6"/>
       <c r="BF30" s="4">
         <v>0.36630471150614557</v>
       </c>
@@ -4448,8 +4448,8 @@
       <c r="BN30" s="6"/>
     </row>
     <row r="31" spans="1:66" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="31"/>
-      <c r="B31" s="31"/>
+      <c r="A31" s="30"/>
+      <c r="B31" s="30"/>
       <c r="C31" s="2">
         <v>4</v>
       </c>
@@ -4540,39 +4540,39 @@
         <v>25.950321534863946</v>
       </c>
       <c r="AN31" s="7">
-        <v>0.17760951977023001</v>
+        <v>0.17298645318451839</v>
       </c>
       <c r="AO31" s="8"/>
       <c r="AP31" s="8">
-        <v>0.17824022360643865</v>
+        <v>0.17230666541510456</v>
       </c>
       <c r="AQ31" s="8"/>
       <c r="AR31" s="8">
-        <v>0.17809875650707316</v>
+        <v>0.17312776915789235</v>
       </c>
       <c r="AS31" s="8"/>
       <c r="AT31" s="8">
-        <v>0.17783307377861174</v>
+        <v>0.17311991221352394</v>
       </c>
       <c r="AU31" s="8"/>
       <c r="AV31" s="9"/>
       <c r="AW31" s="7">
-        <v>2.0777218222358389</v>
+        <v>2.0631137185640886</v>
       </c>
       <c r="AX31" s="8"/>
       <c r="AY31" s="8">
-        <v>2.0879569051039955</v>
+        <v>2.0608845303214478</v>
       </c>
       <c r="AZ31" s="8"/>
       <c r="BA31" s="8">
-        <v>2.0833955574139815</v>
+        <v>2.0586601541419318</v>
       </c>
       <c r="BB31" s="8"/>
       <c r="BC31" s="8">
-        <v>2.0743323902256661</v>
+        <v>2.0619985219594592</v>
       </c>
       <c r="BD31" s="8"/>
-      <c r="BE31" s="8"/>
+      <c r="BE31" s="9"/>
       <c r="BF31" s="7">
         <v>0.74578636669110454</v>
       </c>
@@ -4598,8 +4598,8 @@
       <c r="BN31" s="9"/>
     </row>
     <row r="32" spans="1:66" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="31"/>
-      <c r="B32" s="31"/>
+      <c r="A32" s="30"/>
+      <c r="B32" s="30"/>
       <c r="C32" s="2">
         <v>8</v>
       </c>
@@ -4690,39 +4690,39 @@
         <v>27.642733808876812</v>
       </c>
       <c r="AN32" s="7">
-        <v>0.35668043624357176</v>
+        <v>0.34664884961833797</v>
       </c>
       <c r="AO32" s="8"/>
       <c r="AP32" s="8">
-        <v>0.35729848411230269</v>
+        <v>0.34382129478368634</v>
       </c>
       <c r="AQ32" s="8"/>
       <c r="AR32" s="8">
-        <v>0.35623077607741516</v>
+        <v>0.34628697037263984</v>
       </c>
       <c r="AS32" s="8"/>
       <c r="AT32" s="8">
-        <v>0.35686395674493665</v>
+        <v>0.34657011589215952</v>
       </c>
       <c r="AU32" s="8"/>
       <c r="AV32" s="9"/>
       <c r="AW32" s="7">
-        <v>4.093022817194206</v>
+        <v>4.0388536428004231</v>
       </c>
       <c r="AX32" s="8"/>
       <c r="AY32" s="8">
-        <v>4.1084515515616591</v>
+        <v>4.0452781183722166</v>
       </c>
       <c r="AZ32" s="8"/>
       <c r="BA32" s="8">
-        <v>4.104031485341582</v>
+        <v>4.0218210496837115</v>
       </c>
       <c r="BB32" s="8"/>
       <c r="BC32" s="8">
-        <v>4.101825016801075</v>
+        <v>4.0345819837387626</v>
       </c>
       <c r="BD32" s="8"/>
-      <c r="BE32" s="8"/>
+      <c r="BE32" s="9"/>
       <c r="BF32" s="7">
         <v>1.4626906693347395</v>
       </c>
@@ -4748,8 +4748,8 @@
       <c r="BN32" s="9"/>
     </row>
     <row r="33" spans="1:66" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="31"/>
-      <c r="B33" s="31"/>
+      <c r="A33" s="30"/>
+      <c r="B33" s="30"/>
       <c r="C33" s="2">
         <v>16</v>
       </c>
@@ -4840,39 +4840,39 @@
         <v>31.855509525052192</v>
       </c>
       <c r="AN33" s="7">
-        <v>0.71060350498300195</v>
+        <v>0.69213413147509761</v>
       </c>
       <c r="AO33" s="8"/>
       <c r="AP33" s="8">
-        <v>0.71222876505321131</v>
+        <v>0.68897769731792113</v>
       </c>
       <c r="AQ33" s="8"/>
       <c r="AR33" s="8">
-        <v>0.71222876505321131</v>
+        <v>0.69437037827076231</v>
       </c>
       <c r="AS33" s="8"/>
       <c r="AT33" s="8">
-        <v>0.7112991358614581</v>
+        <v>0.69547807942114859</v>
       </c>
       <c r="AU33" s="8"/>
       <c r="AV33" s="9"/>
       <c r="AW33" s="7">
-        <v>8.4912571299387878</v>
+        <v>8.2213303138469822</v>
       </c>
       <c r="AX33" s="8"/>
       <c r="AY33" s="8">
-        <v>8.5054565565774798</v>
+        <v>8.2213303138469822</v>
       </c>
       <c r="AZ33" s="8"/>
       <c r="BA33" s="8">
-        <v>8.4818171553640909</v>
+        <v>8.239086966792657</v>
       </c>
       <c r="BB33" s="8"/>
       <c r="BC33" s="8">
-        <v>8.4771050347222232</v>
+        <v>8.2036500336021501</v>
       </c>
       <c r="BD33" s="8"/>
-      <c r="BE33" s="8"/>
+      <c r="BE33" s="9"/>
       <c r="BF33" s="7">
         <v>2.7281940036652963</v>
       </c>
@@ -4898,8 +4898,8 @@
       <c r="BN33" s="9"/>
     </row>
     <row r="34" spans="1:66" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="31"/>
-      <c r="B34" s="31"/>
+      <c r="A34" s="30"/>
+      <c r="B34" s="30"/>
       <c r="C34" s="2">
         <v>32</v>
       </c>
@@ -4990,39 +4990,39 @@
         <v>33.135263979370251</v>
       </c>
       <c r="AN34" s="7">
-        <v>1.4193562218036371</v>
+        <v>1.3855252031689822</v>
       </c>
       <c r="AO34" s="8"/>
       <c r="AP34" s="8">
-        <v>1.4222004904930561</v>
+        <v>1.3824497451868629</v>
       </c>
       <c r="AQ34" s="8"/>
       <c r="AR34" s="8">
-        <v>1.426388320869362</v>
+        <v>1.385902730472298</v>
       </c>
       <c r="AS34" s="8"/>
       <c r="AT34" s="8">
-        <v>1.419158208937872</v>
+        <v>1.3852107541645864</v>
       </c>
       <c r="AU34" s="8"/>
       <c r="AV34" s="9"/>
       <c r="AW34" s="7">
-        <v>16.639900831515813</v>
+        <v>16.20689225969198</v>
       </c>
       <c r="AX34" s="8"/>
       <c r="AY34" s="8">
-        <v>16.639900831515813</v>
+        <v>16.22412446836789</v>
       </c>
       <c r="AZ34" s="8"/>
       <c r="BA34" s="8">
-        <v>16.667164459311852</v>
+        <v>15.75507389003614</v>
       </c>
       <c r="BB34" s="8"/>
       <c r="BC34" s="8">
-        <v>16.694517573851204</v>
+        <v>16.155414571201693</v>
       </c>
       <c r="BD34" s="8"/>
-      <c r="BE34" s="8"/>
+      <c r="BE34" s="9"/>
       <c r="BF34" s="7">
         <v>5.4340416889245011</v>
       </c>
@@ -5048,8 +5048,8 @@
       <c r="BN34" s="9"/>
     </row>
     <row r="35" spans="1:66" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="31"/>
-      <c r="B35" s="31"/>
+      <c r="A35" s="30"/>
+      <c r="B35" s="30"/>
       <c r="C35" s="2">
         <v>64</v>
       </c>
@@ -5140,39 +5140,39 @@
         <v>33.11728499728703</v>
       </c>
       <c r="AN35" s="7">
-        <v>2.8601291588566076</v>
+        <v>2.7626468225229712</v>
       </c>
       <c r="AO35" s="8"/>
       <c r="AP35" s="8">
-        <v>2.8383164178757441</v>
+        <v>2.7537969793358599</v>
       </c>
       <c r="AQ35" s="8"/>
       <c r="AR35" s="8">
-        <v>2.8469217897289987</v>
+        <v>2.7697928957161007</v>
       </c>
       <c r="AS35" s="8"/>
       <c r="AT35" s="8">
-        <v>2.8323892640029702</v>
+        <v>2.7690389370293076</v>
       </c>
       <c r="AU35" s="8"/>
       <c r="AV35" s="9"/>
       <c r="AW35" s="7">
-        <v>32.174568397469692</v>
+        <v>31.300080128205128</v>
       </c>
       <c r="AX35" s="8"/>
       <c r="AY35" s="8">
-        <v>32.157616570073763</v>
+        <v>31.332215734086244</v>
       </c>
       <c r="AZ35" s="8"/>
       <c r="BA35" s="8">
-        <v>32.191538106540087</v>
+        <v>31.252000128008188</v>
       </c>
       <c r="BB35" s="8"/>
       <c r="BC35" s="8">
-        <v>32.106868095739081</v>
+        <v>31.284037032291131</v>
       </c>
       <c r="BD35" s="8"/>
-      <c r="BE35" s="8"/>
+      <c r="BE35" s="9"/>
       <c r="BF35" s="7">
         <v>9.7985481216888743</v>
       </c>
@@ -5198,8 +5198,8 @@
       <c r="BN35" s="9"/>
     </row>
     <row r="36" spans="1:66" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="31"/>
-      <c r="B36" s="31"/>
+      <c r="A36" s="30"/>
+      <c r="B36" s="30"/>
       <c r="C36" s="2">
         <v>128</v>
       </c>
@@ -5290,39 +5290,39 @@
         <v>34.318333567613159</v>
       </c>
       <c r="AN36" s="7">
-        <v>5.5645855176186352</v>
+        <v>5.4342835996972791</v>
       </c>
       <c r="AO36" s="8"/>
       <c r="AP36" s="8">
-        <v>5.5788269503221972</v>
+        <v>5.3780206405850741</v>
       </c>
       <c r="AQ36" s="8"/>
       <c r="AR36" s="8">
-        <v>5.5704258693072921</v>
+        <v>5.4246239390303508</v>
       </c>
       <c r="AS36" s="8"/>
       <c r="AT36" s="8">
-        <v>5.6529736269334077</v>
+        <v>5.433799799688404</v>
       </c>
       <c r="AU36" s="8"/>
       <c r="AV36" s="9"/>
       <c r="AW36" s="7">
-        <v>60.490739593657089</v>
+        <v>58.914243484555989</v>
       </c>
       <c r="AX36" s="8"/>
       <c r="AY36" s="8">
-        <v>60.580800248138949</v>
+        <v>58.857431292189005</v>
       </c>
       <c r="AZ36" s="8"/>
       <c r="BA36" s="8">
-        <v>60.460778850916292</v>
+        <v>58.687650240384613</v>
       </c>
       <c r="BB36" s="8"/>
       <c r="BC36" s="8">
-        <v>60.671129473161038</v>
+        <v>58.715879028379028</v>
       </c>
       <c r="BD36" s="8"/>
-      <c r="BE36" s="8"/>
+      <c r="BE36" s="9"/>
       <c r="BF36" s="7">
         <v>16.198289875265392</v>
       </c>
@@ -5348,8 +5348,8 @@
       <c r="BN36" s="9"/>
     </row>
     <row r="37" spans="1:66" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="31"/>
-      <c r="B37" s="31"/>
+      <c r="A37" s="30"/>
+      <c r="B37" s="30"/>
       <c r="C37" s="2">
         <v>256</v>
       </c>
@@ -5440,39 +5440,39 @@
         <v>34.85731367789834</v>
       </c>
       <c r="AN37" s="7">
-        <v>11.180135778724184</v>
+        <v>10.844428774485852</v>
       </c>
       <c r="AO37" s="8"/>
       <c r="AP37" s="8">
-        <v>11.18115983512709</v>
+        <v>10.795040015917934</v>
       </c>
       <c r="AQ37" s="8"/>
       <c r="AR37" s="8">
-        <v>11.151028820681464</v>
+        <v>10.84105794849023</v>
       </c>
       <c r="AS37" s="8"/>
       <c r="AT37" s="8">
-        <v>11.160204104955202</v>
+        <v>10.882616787019703</v>
       </c>
       <c r="AU37" s="8"/>
       <c r="AV37" s="9"/>
       <c r="AW37" s="7">
-        <v>107.45626100352112</v>
+        <v>104.69152015437393</v>
       </c>
       <c r="AX37" s="8"/>
       <c r="AY37" s="8">
-        <v>107.45626100352112</v>
+        <v>104.87140249140893</v>
       </c>
       <c r="AZ37" s="8"/>
       <c r="BA37" s="8">
-        <v>107.55093612334802</v>
+        <v>104.69152015437393</v>
       </c>
       <c r="BB37" s="8"/>
       <c r="BC37" s="8">
-        <v>107.40898592168939</v>
+        <v>104.87140249140893</v>
       </c>
       <c r="BD37" s="8"/>
-      <c r="BE37" s="8"/>
+      <c r="BE37" s="9"/>
       <c r="BF37" s="7">
         <v>21.115777979588305</v>
       </c>
@@ -5498,8 +5498,8 @@
       <c r="BN37" s="9"/>
     </row>
     <row r="38" spans="1:66" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="31"/>
-      <c r="B38" s="31"/>
+      <c r="A38" s="30"/>
+      <c r="B38" s="30"/>
       <c r="C38" s="2">
         <v>512</v>
       </c>
@@ -5590,39 +5590,39 @@
         <v>35.087758695027304</v>
       </c>
       <c r="AN38" s="7">
-        <v>20.358624499666444</v>
+        <v>19.842378494798439</v>
       </c>
       <c r="AO38" s="8"/>
       <c r="AP38" s="8">
-        <v>21.452539431483679</v>
+        <v>20.886356831208829</v>
       </c>
       <c r="AQ38" s="8"/>
       <c r="AR38" s="8">
-        <v>21.798270089285715</v>
+        <v>21.227773671854621</v>
       </c>
       <c r="AS38" s="8"/>
       <c r="AT38" s="8">
-        <v>21.929455223210276</v>
+        <v>21.290714659457574</v>
       </c>
       <c r="AU38" s="8"/>
       <c r="AV38" s="9"/>
       <c r="AW38" s="7">
-        <v>113.23776669758811</v>
+        <v>111.5561457619374</v>
       </c>
       <c r="AX38" s="8"/>
       <c r="AY38" s="8">
-        <v>154.86243260386934</v>
+        <v>152.06516661476175</v>
       </c>
       <c r="AZ38" s="8"/>
       <c r="BA38" s="8">
-        <v>174.38616071428572</v>
+        <v>170.42975567190226</v>
       </c>
       <c r="BB38" s="8"/>
       <c r="BC38" s="8">
-        <v>175.51446800862689</v>
+        <v>172.53754416961129</v>
       </c>
       <c r="BD38" s="8"/>
-      <c r="BE38" s="8"/>
+      <c r="BE38" s="9"/>
       <c r="BF38" s="7">
         <v>29.977974582514733</v>
       </c>
@@ -5648,8 +5648,8 @@
       <c r="BN38" s="9"/>
     </row>
     <row r="39" spans="1:66" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="31"/>
-      <c r="B39" s="31"/>
+      <c r="A39" s="30"/>
+      <c r="B39" s="30"/>
       <c r="C39" s="2">
         <v>1024</v>
       </c>
@@ -5740,39 +5740,39 @@
         <v>35.181299084948485</v>
       </c>
       <c r="AN39" s="7">
-        <v>34.317127596022068</v>
+        <v>33.651361130254998</v>
       </c>
       <c r="AO39" s="8"/>
       <c r="AP39" s="8">
-        <v>38.865065467425481</v>
+        <v>37.667303093419733</v>
       </c>
       <c r="AQ39" s="8"/>
       <c r="AR39" s="8">
-        <v>40.504458730817085</v>
+        <v>39.367995646214624</v>
       </c>
       <c r="AS39" s="8"/>
       <c r="AT39" s="8">
-        <v>41.464100713315219</v>
+        <v>40.312177502579978</v>
       </c>
       <c r="AU39" s="8"/>
       <c r="AV39" s="9"/>
       <c r="AW39" s="7">
-        <v>111.06135562379164</v>
+        <v>110.34604519774011</v>
       </c>
       <c r="AX39" s="8"/>
       <c r="AY39" s="8">
-        <v>181.41603195244286</v>
+        <v>179.84576427255988</v>
       </c>
       <c r="AZ39" s="8"/>
       <c r="BA39" s="8">
-        <v>224.23938002296211</v>
+        <v>220.89176656864964</v>
       </c>
       <c r="BB39" s="8"/>
       <c r="BC39" s="8">
-        <v>257.87232637972011</v>
+        <v>254.37939567595728</v>
       </c>
       <c r="BD39" s="8"/>
-      <c r="BE39" s="8"/>
+      <c r="BE39" s="9"/>
       <c r="BF39" s="7">
         <v>37.32038445370123</v>
       </c>
@@ -5798,8 +5798,8 @@
       <c r="BN39" s="9"/>
     </row>
     <row r="40" spans="1:66" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="31"/>
-      <c r="B40" s="31"/>
+      <c r="A40" s="30"/>
+      <c r="B40" s="30"/>
       <c r="C40" s="2">
         <v>2048</v>
       </c>
@@ -5890,39 +5890,39 @@
         <v>35.250509863374667</v>
       </c>
       <c r="AN40" s="7">
-        <v>51.976608031508633</v>
+        <v>51.303519831888629</v>
       </c>
       <c r="AO40" s="8"/>
       <c r="AP40" s="8">
-        <v>66.140365729766344</v>
+        <v>64.222182033407861</v>
       </c>
       <c r="AQ40" s="8"/>
       <c r="AR40" s="8">
-        <v>71.54041976484379</v>
+        <v>69.881748899781741</v>
       </c>
       <c r="AS40" s="8"/>
       <c r="AT40" s="8">
-        <v>76.168980578738015</v>
+        <v>74.243547344813166</v>
       </c>
       <c r="AU40" s="8"/>
       <c r="AV40" s="9"/>
       <c r="AW40" s="7">
-        <v>110.01042018700011</v>
+        <v>109.7322883308051</v>
       </c>
       <c r="AX40" s="8"/>
       <c r="AY40" s="8">
-        <v>197.18576476527008</v>
+        <v>196.90745034781733</v>
       </c>
       <c r="AZ40" s="8"/>
       <c r="BA40" s="8">
-        <v>260.7295421172073</v>
+        <v>258.45242821225355</v>
       </c>
       <c r="BB40" s="8"/>
       <c r="BC40" s="8">
-        <v>330.25448089279678</v>
+        <v>326.4457629951529</v>
       </c>
       <c r="BD40" s="8"/>
-      <c r="BE40" s="8"/>
+      <c r="BE40" s="9"/>
       <c r="BF40" s="7">
         <v>42.516544037615915</v>
       </c>
@@ -5948,8 +5948,8 @@
       <c r="BN40" s="9"/>
     </row>
     <row r="41" spans="1:66" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="31"/>
-      <c r="B41" s="31"/>
+      <c r="A41" s="30"/>
+      <c r="B41" s="30"/>
       <c r="C41" s="2">
         <v>4096</v>
       </c>
@@ -6040,39 +6040,39 @@
         <v>35.262283687046953</v>
       </c>
       <c r="AN41" s="7">
-        <v>70.5392130306806</v>
+        <v>69.760692919010623</v>
       </c>
       <c r="AO41" s="8"/>
       <c r="AP41" s="8">
-        <v>101.32155733665343</v>
+        <v>99.524828658054972</v>
       </c>
       <c r="AQ41" s="8"/>
       <c r="AR41" s="8">
-        <v>116.41682064731478</v>
+        <v>114.27463944065764</v>
       </c>
       <c r="AS41" s="8"/>
       <c r="AT41" s="8">
-        <v>129.66374560180574</v>
+        <v>127.43035166699288</v>
       </c>
       <c r="AU41" s="8"/>
       <c r="AV41" s="9"/>
       <c r="AW41" s="7">
-        <v>109.53228836609371</v>
+        <v>109.38200044802868</v>
       </c>
       <c r="AX41" s="8"/>
       <c r="AY41" s="8">
-        <v>207.58050802423213</v>
+        <v>206.90979395095079</v>
       </c>
       <c r="AZ41" s="8"/>
       <c r="BA41" s="8">
-        <v>283.61649604298265</v>
+        <v>282.48842927393696</v>
       </c>
       <c r="BB41" s="8"/>
       <c r="BC41" s="8">
-        <v>375.56484953369869</v>
+        <v>373.44646271510516</v>
       </c>
       <c r="BD41" s="8"/>
-      <c r="BE41" s="8"/>
+      <c r="BE41" s="9"/>
       <c r="BF41" s="7">
         <v>43.275835327483826</v>
       </c>
@@ -6098,8 +6098,8 @@
       <c r="BN41" s="9"/>
     </row>
     <row r="42" spans="1:66" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="31"/>
-      <c r="B42" s="31"/>
+      <c r="A42" s="30"/>
+      <c r="B42" s="30"/>
       <c r="C42" s="2">
         <v>8192</v>
       </c>
@@ -6190,39 +6190,39 @@
         <v>35.262283687046953</v>
       </c>
       <c r="AN42" s="7">
-        <v>85.697205037076046</v>
+        <v>85.152648042987778</v>
       </c>
       <c r="AO42" s="8"/>
       <c r="AP42" s="8">
-        <v>138.27433628318585</v>
+        <v>136.58694359942655</v>
       </c>
       <c r="AQ42" s="8"/>
       <c r="AR42" s="8">
-        <v>169.65255157437568</v>
+        <v>167.47052518756698</v>
       </c>
       <c r="AS42" s="8"/>
       <c r="AT42" s="8">
-        <v>199.65499616662407</v>
+        <v>196.88263904639498</v>
       </c>
       <c r="AU42" s="8"/>
       <c r="AV42" s="9"/>
       <c r="AW42" s="7">
-        <v>109.25809383959164</v>
+        <v>109.18785202163491</v>
       </c>
       <c r="AX42" s="8"/>
       <c r="AY42" s="8">
-        <v>212.60817503946009</v>
+        <v>212.3539005164447</v>
       </c>
       <c r="AZ42" s="8"/>
       <c r="BA42" s="8">
-        <v>296.69223758164969</v>
+        <v>296.17484267192356</v>
       </c>
       <c r="BB42" s="8"/>
       <c r="BC42" s="8">
-        <v>402.85154437168052</v>
+        <v>402.18790218790218</v>
       </c>
       <c r="BD42" s="8"/>
-      <c r="BE42" s="8"/>
+      <c r="BE42" s="9"/>
       <c r="BF42" s="7">
         <v>47.43271384944174</v>
       </c>
@@ -6248,8 +6248,8 @@
       <c r="BN42" s="9"/>
     </row>
     <row r="43" spans="1:66" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="31"/>
-      <c r="B43" s="31"/>
+      <c r="A43" s="30"/>
+      <c r="B43" s="30"/>
       <c r="C43" s="2">
         <v>16384</v>
       </c>
@@ -6340,39 +6340,39 @@
         <v>35.222697619058358</v>
       </c>
       <c r="AN43" s="7">
-        <v>95.997886510530577</v>
+        <v>95.566333739044268</v>
       </c>
       <c r="AO43" s="8"/>
       <c r="AP43" s="8">
-        <v>169.39505637467477</v>
+        <v>167.86454808177825</v>
       </c>
       <c r="AQ43" s="8"/>
       <c r="AR43" s="8">
-        <v>219.52932911837024</v>
+        <v>218.08310187446787</v>
       </c>
       <c r="AS43" s="8"/>
       <c r="AT43" s="8">
-        <v>274.33939074708104</v>
+        <v>270.92400256619214</v>
       </c>
       <c r="AU43" s="8"/>
       <c r="AV43" s="9"/>
       <c r="AW43" s="7">
-        <v>109.08875111706881</v>
+        <v>109.11693844058802</v>
       </c>
       <c r="AX43" s="8"/>
       <c r="AY43" s="8">
-        <v>215.00123840713323</v>
+        <v>215.14629948364887</v>
       </c>
       <c r="AZ43" s="8"/>
       <c r="BA43" s="8">
-        <v>303.30382793695162</v>
+        <v>303.6574937810945</v>
       </c>
       <c r="BB43" s="8"/>
       <c r="BC43" s="8">
-        <v>417.91483898577081</v>
+        <v>418.46326896810302</v>
       </c>
       <c r="BD43" s="8"/>
-      <c r="BE43" s="8"/>
+      <c r="BE43" s="9"/>
       <c r="BF43" s="7">
         <v>48.027417892326369</v>
       </c>
@@ -6398,8 +6398,8 @@
       <c r="BN43" s="9"/>
     </row>
     <row r="44" spans="1:66" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="31"/>
-      <c r="B44" s="31"/>
+      <c r="A44" s="30"/>
+      <c r="B44" s="30"/>
       <c r="C44" s="2">
         <v>32768</v>
       </c>
@@ -6490,39 +6490,39 @@
         <v>34.837612135305939</v>
       </c>
       <c r="AN44" s="7">
-        <v>102.10482980350129</v>
+        <v>101.88844112315297</v>
       </c>
       <c r="AO44" s="8"/>
       <c r="AP44" s="8">
-        <v>190.76397155327658</v>
+        <v>189.93034874250912</v>
       </c>
       <c r="AQ44" s="8"/>
       <c r="AR44" s="8">
-        <v>257.79361661758276</v>
+        <v>256.38711582954562</v>
       </c>
       <c r="AS44" s="8"/>
       <c r="AT44" s="8">
-        <v>336.84369374710315</v>
+        <v>334.24247285951122</v>
       </c>
       <c r="AU44" s="8"/>
       <c r="AV44" s="9"/>
       <c r="AW44" s="7">
-        <v>109.02861608669258</v>
+        <v>109.03926809354</v>
       </c>
       <c r="AX44" s="8"/>
       <c r="AY44" s="8">
-        <v>216.40974501738205</v>
+        <v>216.44721804719589</v>
       </c>
       <c r="AZ44" s="8"/>
       <c r="BA44" s="8">
-        <v>307.13134410504381</v>
+        <v>307.21588674793554</v>
       </c>
       <c r="BB44" s="8"/>
       <c r="BC44" s="8">
-        <v>426.28362525235991</v>
+        <v>426.48724632538585</v>
       </c>
       <c r="BD44" s="8"/>
-      <c r="BE44" s="8"/>
+      <c r="BE44" s="9"/>
       <c r="BF44" s="7">
         <v>48.730511693763432</v>
       </c>
@@ -6548,8 +6548,8 @@
       <c r="BN44" s="9"/>
     </row>
     <row r="45" spans="1:66" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="31"/>
-      <c r="B45" s="31"/>
+      <c r="A45" s="30"/>
+      <c r="B45" s="30"/>
       <c r="C45" s="2">
         <v>65536</v>
       </c>
@@ -6640,39 +6640,39 @@
         <v>34.655298989285136</v>
       </c>
       <c r="AN45" s="7">
-        <v>105.44625699530468</v>
+        <v>101.86419628334218</v>
       </c>
       <c r="AO45" s="8"/>
       <c r="AP45" s="8">
-        <v>203.46840379851093</v>
+        <v>189.74237539238723</v>
       </c>
       <c r="AQ45" s="8"/>
       <c r="AR45" s="8">
-        <v>282.12628423884587</v>
+        <v>256.32823137621602</v>
       </c>
       <c r="AS45" s="8"/>
       <c r="AT45" s="8">
-        <v>380.0870855530419</v>
+        <v>334.49469892801142</v>
       </c>
       <c r="AU45" s="8"/>
       <c r="AV45" s="9"/>
       <c r="AW45" s="7">
-        <v>109.03375161588021</v>
+        <v>109.05639175149801</v>
       </c>
       <c r="AX45" s="8"/>
       <c r="AY45" s="8">
-        <v>217.22658992485697</v>
+        <v>216.50945193663375</v>
       </c>
       <c r="AZ45" s="8"/>
       <c r="BA45" s="8">
-        <v>309.32325022023815</v>
+        <v>307.3715064154581</v>
       </c>
       <c r="BB45" s="8"/>
       <c r="BC45" s="8">
-        <v>431.1831666091756</v>
+        <v>426.734762155113</v>
       </c>
       <c r="BD45" s="8"/>
-      <c r="BE45" s="8"/>
+      <c r="BE45" s="9"/>
       <c r="BF45" s="7">
         <v>49.006462580233375</v>
       </c>
@@ -6698,8 +6698,8 @@
       <c r="BN45" s="9"/>
     </row>
     <row r="46" spans="1:66" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="31"/>
-      <c r="B46" s="31"/>
+      <c r="A46" s="30"/>
+      <c r="B46" s="30"/>
       <c r="C46" s="2">
         <v>131072</v>
       </c>
@@ -6790,39 +6790,39 @@
         <v>34.52543682273177</v>
       </c>
       <c r="AN46" s="7">
-        <v>107.21717396115135</v>
+        <v>101.86087597093787</v>
       </c>
       <c r="AO46" s="8"/>
       <c r="AP46" s="8">
-        <v>210.52277014281864</v>
+        <v>189.70638005320885</v>
       </c>
       <c r="AQ46" s="8"/>
       <c r="AR46" s="8">
-        <v>296.08294112213065</v>
+        <v>256.31088665112395</v>
       </c>
       <c r="AS46" s="8"/>
       <c r="AT46" s="8">
-        <v>406.27021194304416</v>
+        <v>334.42310676390798</v>
       </c>
       <c r="AU46" s="8"/>
       <c r="AV46" s="9"/>
       <c r="AW46" s="7">
-        <v>109.03974367809374</v>
+        <v>109.06076866029751</v>
       </c>
       <c r="AX46" s="8"/>
       <c r="AY46" s="8">
-        <v>217.66688955756157</v>
+        <v>216.532330009129</v>
       </c>
       <c r="AZ46" s="8"/>
       <c r="BA46" s="8">
-        <v>310.43560323846424</v>
+        <v>307.40930195954985</v>
       </c>
       <c r="BB46" s="8"/>
       <c r="BC46" s="8">
-        <v>433.66789365769381</v>
+        <v>426.81344496496718</v>
       </c>
       <c r="BD46" s="8"/>
-      <c r="BE46" s="8"/>
+      <c r="BE46" s="9"/>
       <c r="BF46" s="7">
         <v>48.986316358333731</v>
       </c>
@@ -6848,8 +6848,8 @@
       <c r="BN46" s="9"/>
     </row>
     <row r="47" spans="1:66" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="31"/>
-      <c r="B47" s="31"/>
+      <c r="A47" s="30"/>
+      <c r="B47" s="30"/>
       <c r="C47" s="2">
         <v>262144</v>
       </c>
@@ -6940,39 +6940,39 @@
         <v>34.531927322171967</v>
       </c>
       <c r="AN47" s="7">
-        <v>107.23354608468875</v>
+        <v>101.85768037467328</v>
       </c>
       <c r="AO47" s="8"/>
       <c r="AP47" s="8">
-        <v>210.55326660759945</v>
+        <v>189.73906325065516</v>
       </c>
       <c r="AQ47" s="8"/>
       <c r="AR47" s="8">
-        <v>296.16607097797589</v>
+        <v>256.28119582856226</v>
       </c>
       <c r="AS47" s="8"/>
       <c r="AT47" s="8">
-        <v>406.38644424865652</v>
+        <v>334.55154703326383</v>
       </c>
       <c r="AU47" s="8"/>
       <c r="AV47" s="9"/>
       <c r="AW47" s="7">
-        <v>109.04906597294013</v>
+        <v>109.06305240436043</v>
       </c>
       <c r="AX47" s="8"/>
       <c r="AY47" s="8">
-        <v>217.70252430430983</v>
+        <v>216.53814406022877</v>
       </c>
       <c r="AZ47" s="8"/>
       <c r="BA47" s="8">
-        <v>310.51117591824362</v>
+        <v>307.41761822666763</v>
       </c>
       <c r="BB47" s="8"/>
       <c r="BC47" s="8">
-        <v>433.80936681184818</v>
+        <v>426.8389502493593</v>
       </c>
       <c r="BD47" s="8"/>
-      <c r="BE47" s="8"/>
+      <c r="BE47" s="9"/>
       <c r="BF47" s="7">
         <v>48.999479625526376</v>
       </c>
@@ -6998,8 +6998,8 @@
       <c r="BN47" s="9"/>
     </row>
     <row r="48" spans="1:66" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="31"/>
-      <c r="B48" s="31"/>
+      <c r="A48" s="30"/>
+      <c r="B48" s="30"/>
       <c r="C48" s="2">
         <v>524288</v>
       </c>
@@ -7090,39 +7090,39 @@
         <v>34.479536567444903</v>
       </c>
       <c r="AN48" s="7">
-        <v>107.22821079865288</v>
+        <v>101.84595798854234</v>
       </c>
       <c r="AO48" s="8"/>
       <c r="AP48" s="8">
-        <v>210.56647857465026</v>
+        <v>189.67615452081733</v>
       </c>
       <c r="AQ48" s="8"/>
       <c r="AR48" s="8">
-        <v>296.19572139356535</v>
+        <v>256.1844199907876</v>
       </c>
       <c r="AS48" s="8"/>
       <c r="AT48" s="8">
-        <v>406.42971814099047</v>
+        <v>334.28560158371147</v>
       </c>
       <c r="AU48" s="8"/>
       <c r="AV48" s="9"/>
       <c r="AW48" s="7">
-        <v>109.04930380743464</v>
+        <v>109.05841364940206</v>
       </c>
       <c r="AX48" s="8"/>
       <c r="AY48" s="8">
-        <v>217.69892239033416</v>
+        <v>216.52267187244908</v>
       </c>
       <c r="AZ48" s="8"/>
       <c r="BA48" s="8">
-        <v>310.50114885425074</v>
+        <v>307.38227719856712</v>
       </c>
       <c r="BB48" s="8"/>
       <c r="BC48" s="8">
-        <v>433.79318302688739</v>
+        <v>426.79595738869165</v>
       </c>
       <c r="BD48" s="8"/>
-      <c r="BE48" s="8"/>
+      <c r="BE48" s="9"/>
       <c r="BF48" s="7">
         <v>48.699214754381615</v>
       </c>
@@ -7148,8 +7148,8 @@
       <c r="BN48" s="9"/>
     </row>
     <row r="49" spans="1:66" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="31"/>
-      <c r="B49" s="31"/>
+      <c r="A49" s="30"/>
+      <c r="B49" s="30"/>
       <c r="C49" s="2">
         <v>1048576</v>
       </c>
@@ -7240,39 +7240,39 @@
         <v>34.503303553302011</v>
       </c>
       <c r="AN49" s="7">
-        <v>107.21961106729404</v>
+        <v>101.86176828362717</v>
       </c>
       <c r="AO49" s="8"/>
       <c r="AP49" s="8">
-        <v>210.52135191759689</v>
+        <v>189.74835194068922</v>
       </c>
       <c r="AQ49" s="8"/>
       <c r="AR49" s="8">
-        <v>296.10135193955267</v>
+        <v>256.27003070627507</v>
       </c>
       <c r="AS49" s="8"/>
       <c r="AT49" s="8">
-        <v>406.27235767568334</v>
+        <v>334.49212555362629</v>
       </c>
       <c r="AU49" s="8"/>
       <c r="AV49" s="9"/>
       <c r="AW49" s="7">
-        <v>109.0483643672256</v>
+        <v>109.05715292779195</v>
       </c>
       <c r="AX49" s="8"/>
       <c r="AY49" s="8">
-        <v>217.70010721730281</v>
+        <v>216.52135918251926</v>
       </c>
       <c r="AZ49" s="8"/>
       <c r="BA49" s="8">
-        <v>310.50394479736667</v>
+        <v>307.37377388601595</v>
       </c>
       <c r="BB49" s="8"/>
       <c r="BC49" s="8">
-        <v>433.78546792655317</v>
+        <v>426.74714548834379</v>
       </c>
       <c r="BD49" s="8"/>
-      <c r="BE49" s="8"/>
+      <c r="BE49" s="9"/>
       <c r="BF49" s="7">
         <v>48.366856804841909</v>
       </c>
@@ -7297,9 +7297,9 @@
       </c>
       <c r="BN49" s="9"/>
     </row>
-    <row r="50" spans="1:66" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="32"/>
-      <c r="B50" s="32"/>
+    <row r="50" spans="1:66" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="31"/>
+      <c r="B50" s="31"/>
       <c r="C50" s="2">
         <v>2097152</v>
       </c>
@@ -7390,39 +7390,39 @@
         <v>34.471359298769819</v>
       </c>
       <c r="AN50" s="10">
-        <v>107.22837751830535</v>
+        <v>101.86332986845217</v>
       </c>
       <c r="AO50" s="11"/>
       <c r="AP50" s="11">
-        <v>210.54912158380102</v>
+        <v>189.76574367771704</v>
       </c>
       <c r="AQ50" s="11"/>
       <c r="AR50" s="11">
-        <v>296.15216890742801</v>
+        <v>256.29055557769624</v>
       </c>
       <c r="AS50" s="11"/>
       <c r="AT50" s="11">
-        <v>406.3722418500015</v>
+        <v>334.51483974732088</v>
       </c>
       <c r="AU50" s="11"/>
       <c r="AV50" s="12"/>
       <c r="AW50" s="10">
-        <v>109.05011839843981</v>
+        <v>109.05750973283745</v>
       </c>
       <c r="AX50" s="11"/>
       <c r="AY50" s="11">
-        <v>217.70617373344533</v>
+        <v>216.52536762488884</v>
       </c>
       <c r="AZ50" s="11"/>
       <c r="BA50" s="11">
-        <v>310.51831095427866</v>
+        <v>307.37684447238843</v>
       </c>
       <c r="BB50" s="11"/>
       <c r="BC50" s="11">
-        <v>433.82065853975968</v>
+        <v>426.76116865985472</v>
       </c>
       <c r="BD50" s="11"/>
-      <c r="BE50" s="11"/>
+      <c r="BE50" s="12"/>
       <c r="BF50" s="10">
         <v>48.717224330297718</v>
       </c>
@@ -7453,26 +7453,26 @@
     <row r="54" spans="1:66" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="AW7:BE7"/>
+    <mergeCell ref="BF7:BN7"/>
+    <mergeCell ref="AN5:BN5"/>
+    <mergeCell ref="BF6:BN6"/>
+    <mergeCell ref="AW6:BE6"/>
+    <mergeCell ref="A30:A50"/>
+    <mergeCell ref="B30:B50"/>
+    <mergeCell ref="M6:U6"/>
+    <mergeCell ref="D7:L7"/>
+    <mergeCell ref="M7:U7"/>
+    <mergeCell ref="AE7:AM7"/>
+    <mergeCell ref="AN7:AV7"/>
+    <mergeCell ref="V7:AD7"/>
+    <mergeCell ref="A9:A29"/>
+    <mergeCell ref="B9:B29"/>
     <mergeCell ref="D5:AM5"/>
     <mergeCell ref="D6:L6"/>
     <mergeCell ref="V6:AD6"/>
     <mergeCell ref="AE6:AM6"/>
     <mergeCell ref="AN6:AV6"/>
-    <mergeCell ref="AE7:AM7"/>
-    <mergeCell ref="AN7:AV7"/>
-    <mergeCell ref="V7:AD7"/>
-    <mergeCell ref="A9:A29"/>
-    <mergeCell ref="B9:B29"/>
-    <mergeCell ref="A30:A50"/>
-    <mergeCell ref="B30:B50"/>
-    <mergeCell ref="M6:U6"/>
-    <mergeCell ref="D7:L7"/>
-    <mergeCell ref="M7:U7"/>
-    <mergeCell ref="AW7:BE7"/>
-    <mergeCell ref="BF7:BN7"/>
-    <mergeCell ref="AN5:BN5"/>
-    <mergeCell ref="BF6:BN6"/>
-    <mergeCell ref="AW6:BE6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>